<commit_message>
Process Timer added to GUI Cancel button added to GUI
</commit_message>
<xml_diff>
--- a/ProcessingTimeExtrapolation.xlsx
+++ b/ProcessingTimeExtrapolation.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
+    <sheet name="Forest1 Processing" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Data Set: Forest1.txt</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
   <si>
     <t>No Species</t>
   </si>
@@ -33,16 +31,187 @@
     <t>MSSF Size</t>
   </si>
   <si>
-    <t>MSSF Time</t>
-  </si>
-  <si>
     <t>1-54</t>
+  </si>
+  <si>
+    <t>Species Range</t>
+  </si>
+  <si>
+    <t>Excluded</t>
+  </si>
+  <si>
+    <t>1-30</t>
+  </si>
+  <si>
+    <t>1-35</t>
+  </si>
+  <si>
+    <t>1-40</t>
+  </si>
+  <si>
+    <t>1-45</t>
+  </si>
+  <si>
+    <t>1-50</t>
+  </si>
+  <si>
+    <t>1-51</t>
+  </si>
+  <si>
+    <t>1-52</t>
+  </si>
+  <si>
+    <t>1-53</t>
+  </si>
+  <si>
+    <t>1-55</t>
+  </si>
+  <si>
+    <t>1-56</t>
+  </si>
+  <si>
+    <t>1-57</t>
+  </si>
+  <si>
+    <t>1-58</t>
+  </si>
+  <si>
+    <t>1-59</t>
+  </si>
+  <si>
+    <t>1-60</t>
+  </si>
+  <si>
+    <t>1-61</t>
+  </si>
+  <si>
+    <t>54,57</t>
+  </si>
+  <si>
+    <t>54,57,58</t>
+  </si>
+  <si>
+    <t>1-62</t>
+  </si>
+  <si>
+    <t>1-63</t>
+  </si>
+  <si>
+    <t>1-64</t>
+  </si>
+  <si>
+    <t>1-65</t>
+  </si>
+  <si>
+    <t>1-66</t>
+  </si>
+  <si>
+    <t>1-67</t>
+  </si>
+  <si>
+    <t>1-68</t>
+  </si>
+  <si>
+    <t>1-69</t>
+  </si>
+  <si>
+    <t>1-70</t>
+  </si>
+  <si>
+    <t>1-71</t>
+  </si>
+  <si>
+    <t>1-72</t>
+  </si>
+  <si>
+    <t>1-73</t>
+  </si>
+  <si>
+    <t>1-74</t>
+  </si>
+  <si>
+    <t>1-75</t>
+  </si>
+  <si>
+    <t>1-76</t>
+  </si>
+  <si>
+    <t>1-77</t>
+  </si>
+  <si>
+    <t>1-78</t>
+  </si>
+  <si>
+    <t>1-79</t>
+  </si>
+  <si>
+    <t>54,57,58,69</t>
+  </si>
+  <si>
+    <t>54,57,58,69,70</t>
+  </si>
+  <si>
+    <t>54,57,58,69,70,71</t>
+  </si>
+  <si>
+    <t>54,57,58,69,70,71,72</t>
+  </si>
+  <si>
+    <t>1-80</t>
+  </si>
+  <si>
+    <t>1-81</t>
+  </si>
+  <si>
+    <t>1-82</t>
+  </si>
+  <si>
+    <t>1-83</t>
+  </si>
+  <si>
+    <t>1-84</t>
+  </si>
+  <si>
+    <t>1-85</t>
+  </si>
+  <si>
+    <t>1-86</t>
+  </si>
+  <si>
+    <t>1-87</t>
+  </si>
+  <si>
+    <t>1-88</t>
+  </si>
+  <si>
+    <t>1-89</t>
+  </si>
+  <si>
+    <t>Processing Time ms</t>
+  </si>
+  <si>
+    <t>MSSF Time ms</t>
+  </si>
+  <si>
+    <t>54,57,58,69,70,71,72,78</t>
+  </si>
+  <si>
+    <t>54,57,58,69,70,71,72,78,79</t>
+  </si>
+  <si>
+    <t>54,57,58,69,70,71,72,78,79,82</t>
+  </si>
+  <si>
+    <t>54,57,58,69,70,71,72,78,79,82,88</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="hh:mm:ss;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -52,12 +221,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -72,9 +253,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="17" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -107,6 +317,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Time taken to process subsets of Forest1 dataset</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -139,7 +374,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12113500139130173"/>
+          <c:y val="0.11649782619072292"/>
+          <c:w val="0.7654179545608375"/>
+          <c:h val="0.70780922190378781"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -220,10 +465,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$20</c:f>
+              <c:f>'Forest1 Processing'!$C$2:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>30</c:v>
                 </c:pt>
@@ -252,32 +497,119 @@
                   <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>57</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>58</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>59</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$20</c:f>
+              <c:f>'Forest1 Processing'!$D$2:$D$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>1195</c:v>
                 </c:pt>
@@ -303,25 +635,109 @@
                   <c:v>39038</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>242919</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>43830</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>47562</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>89156</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>135472</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>163843</c:v>
+                  <c:v>82084</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>198760</c:v>
+                  <c:v>55626</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>233032</c:v>
+                  <c:v>73297</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>79340</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>96783</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>120869</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>139989</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>180415</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>244787</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>279875</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>282665</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="0">
+                  <c:v>809061</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="0">
+                  <c:v>595174</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="0">
+                  <c:v>666395</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="0">
+                  <c:v>1930064</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="0">
+                  <c:v>317918</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="0">
+                  <c:v>509197</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="0">
+                  <c:v>664614</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="0">
+                  <c:v>711559</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="0">
+                  <c:v>743164</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="0">
+                  <c:v>1162769</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="0">
+                  <c:v>1435281</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0">
+                  <c:v>1109696</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0">
+                  <c:v>1393977</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2505126</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1614447</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1940835</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2114103</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2364937</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2555695</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="0">
+                  <c:v>3305786</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -329,7 +745,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1EEE-4F29-BA03-E39A74028D38}"/>
+              <c16:uniqueId val="{00000000-8E5D-48D7-A309-C17EAAB1EE56}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -377,12 +793,26 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$A$18</c:f>
+              <c:f>'Forest1 Processing'!$C$2:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>30</c:v>
                 </c:pt>
@@ -411,32 +841,119 @@
                   <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>57</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>58</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>59</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$D$18</c:f>
+              <c:f>'Forest1 Processing'!$G$2:$G$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>117</c:v>
                 </c:pt>
@@ -462,25 +979,109 @@
                   <c:v>976</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>81722</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>1138</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>1107</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>2851</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>8143</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>12443</c:v>
+                  <c:v>3492</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14855</c:v>
+                  <c:v>1549</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17259</c:v>
+                  <c:v>4091</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2924</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4344</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5882</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5875</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9828</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15496</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>17421</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>17682</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>212413</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>165984</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>138154</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1341610</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>18467</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>35294</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>55980</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>59892</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>64117</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>207746</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>349558</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>155955</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>249984</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>700271</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>325120</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>411064</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>491724</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>611868</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>626432</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1002787</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -488,7 +1089,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1EEE-4F29-BA03-E39A74028D38}"/>
+              <c16:uniqueId val="{00000001-8E5D-48D7-A309-C17EAAB1EE56}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -507,6 +1108,7 @@
         <c:axId val="413666096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="45"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -524,6 +1126,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of Species</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -586,6 +1244,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Processing Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -631,9 +1345,66 @@
         <c:axId val="413704400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>MSSF Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -674,6 +1445,7 @@
         <c:crossAx val="490884776"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1500000"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="490884776"/>
@@ -687,6 +1459,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="413704400"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -697,6 +1470,47 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11980837638848155"/>
+          <c:y val="0.92197645574075071"/>
+          <c:w val="0.64332438387894919"/>
+          <c:h val="5.7472232790385706E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -726,11 +1540,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1290,25 +2099,28 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9282839" cy="6054025"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1321,7 +2133,7 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1588,268 +2400,1153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>1195</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2">
+        <v>164</v>
+      </c>
+      <c r="G2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>5869</v>
+      </c>
+      <c r="E3" s="21">
+        <f t="shared" ref="E3:E36" si="0">D3/3600000/24</f>
+        <v>6.7928240740740742E-5</v>
+      </c>
+      <c r="F3">
+        <v>1104</v>
+      </c>
+      <c r="G3">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <v>11469</v>
+      </c>
+      <c r="E4" s="21">
+        <f t="shared" si="0"/>
+        <v>1.3274305555555557E-4</v>
+      </c>
+      <c r="F4">
+        <v>1548</v>
+      </c>
+      <c r="G4">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>45</v>
+      </c>
+      <c r="D5">
+        <v>18602</v>
+      </c>
+      <c r="E5" s="21">
+        <f t="shared" si="0"/>
+        <v>2.1530092592592594E-4</v>
+      </c>
+      <c r="F5">
+        <v>1780</v>
+      </c>
+      <c r="G5">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>30098</v>
+      </c>
+      <c r="E6" s="21">
+        <f t="shared" si="0"/>
+        <v>3.4835648148148144E-4</v>
+      </c>
+      <c r="F6">
+        <v>2084</v>
+      </c>
+      <c r="G6">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>51</v>
+      </c>
+      <c r="D7">
+        <v>32362</v>
+      </c>
+      <c r="E7" s="21">
+        <f t="shared" si="0"/>
+        <v>3.7456018518518518E-4</v>
+      </c>
+      <c r="F7">
+        <v>2150</v>
+      </c>
+      <c r="G7">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>52</v>
+      </c>
+      <c r="D8">
+        <v>37169</v>
+      </c>
+      <c r="E8" s="21">
+        <f t="shared" si="0"/>
+        <v>4.3019675925925929E-4</v>
+      </c>
+      <c r="F8">
+        <v>2290</v>
+      </c>
+      <c r="G8">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>53</v>
+      </c>
+      <c r="D9">
+        <v>39038</v>
+      </c>
+      <c r="E9" s="21">
+        <f t="shared" si="0"/>
+        <v>4.5182870370370369E-4</v>
+      </c>
+      <c r="F9">
+        <v>2348</v>
+      </c>
+      <c r="G9">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4">
+        <v>54</v>
+      </c>
+      <c r="D10" s="4">
+        <v>242919</v>
+      </c>
+      <c r="E10" s="20">
+        <f t="shared" si="0"/>
+        <v>2.8115624999999998E-3</v>
+      </c>
+      <c r="F10" s="4">
+        <v>9974</v>
+      </c>
+      <c r="G10" s="4">
+        <v>81722</v>
+      </c>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>54</v>
+      </c>
+      <c r="C11">
+        <v>54</v>
+      </c>
+      <c r="D11">
+        <v>43830</v>
+      </c>
+      <c r="E11" s="21">
+        <f t="shared" si="0"/>
+        <v>5.0729166666666663E-4</v>
+      </c>
+      <c r="F11">
+        <v>2416</v>
+      </c>
+      <c r="G11">
+        <v>1138</v>
+      </c>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>54</v>
+      </c>
+      <c r="C12">
+        <v>55</v>
+      </c>
+      <c r="D12">
+        <v>47562</v>
+      </c>
+      <c r="E12" s="21">
+        <f t="shared" si="0"/>
+        <v>5.5048611111111108E-4</v>
+      </c>
+      <c r="F12">
+        <v>2556</v>
+      </c>
+      <c r="G12">
+        <v>1107</v>
+      </c>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4">
+        <v>54</v>
+      </c>
+      <c r="C13" s="4">
+        <v>56</v>
+      </c>
+      <c r="D13" s="4">
+        <v>89156</v>
+      </c>
+      <c r="E13" s="20">
+        <f t="shared" si="0"/>
+        <v>1.0318981481481481E-3</v>
+      </c>
+      <c r="F13" s="4">
+        <v>4688</v>
+      </c>
+      <c r="G13" s="4">
+        <v>2851</v>
+      </c>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="4">
+        <v>56</v>
+      </c>
+      <c r="D14" s="4">
+        <v>82084</v>
+      </c>
+      <c r="E14" s="20">
+        <f t="shared" si="0"/>
+        <v>9.5004629629629638E-4</v>
+      </c>
+      <c r="F14" s="4">
+        <v>4056</v>
+      </c>
+      <c r="G14" s="4">
+        <v>3492</v>
+      </c>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>56</v>
+      </c>
+      <c r="D15">
+        <v>55626</v>
+      </c>
+      <c r="E15" s="21">
+        <f t="shared" si="0"/>
+        <v>6.4381944444444447E-4</v>
+      </c>
+      <c r="F15">
+        <v>2790</v>
+      </c>
+      <c r="G15">
+        <v>1549</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>57</v>
+      </c>
+      <c r="D16">
+        <v>73297</v>
+      </c>
+      <c r="E16" s="21">
+        <f t="shared" si="0"/>
+        <v>8.4834490740740747E-4</v>
+      </c>
+      <c r="F16">
+        <v>3328</v>
+      </c>
+      <c r="G16">
+        <v>4091</v>
+      </c>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <v>58</v>
+      </c>
+      <c r="D17">
+        <v>79340</v>
+      </c>
+      <c r="E17" s="21">
+        <f t="shared" si="0"/>
+        <v>9.1828703703703701E-4</v>
+      </c>
+      <c r="F17">
+        <v>3554</v>
+      </c>
+      <c r="G17">
+        <v>2924</v>
+      </c>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>59</v>
+      </c>
+      <c r="D18">
+        <v>96783</v>
+      </c>
+      <c r="E18" s="21">
+        <f t="shared" si="0"/>
+        <v>1.1201736111111111E-3</v>
+      </c>
+      <c r="F18">
+        <v>4040</v>
+      </c>
+      <c r="G18">
+        <v>4344</v>
+      </c>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19">
+        <v>60</v>
+      </c>
+      <c r="D19">
+        <v>120869</v>
+      </c>
+      <c r="E19" s="21">
+        <f t="shared" si="0"/>
+        <v>1.3989467592592593E-3</v>
+      </c>
+      <c r="F19">
+        <v>4866</v>
+      </c>
+      <c r="G19">
+        <v>5882</v>
+      </c>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>61</v>
+      </c>
+      <c r="D20">
+        <v>139989</v>
+      </c>
+      <c r="E20" s="21">
+        <f t="shared" si="0"/>
+        <v>1.6202430555555555E-3</v>
+      </c>
+      <c r="F20">
+        <v>5004</v>
+      </c>
+      <c r="G20">
+        <v>5875</v>
+      </c>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>62</v>
+      </c>
+      <c r="D21">
+        <v>180415</v>
+      </c>
+      <c r="E21" s="21">
+        <f t="shared" si="0"/>
+        <v>2.0881365740740743E-3</v>
+      </c>
+      <c r="F21">
+        <v>6404</v>
+      </c>
+      <c r="G21">
+        <v>9828</v>
+      </c>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22">
+        <v>63</v>
+      </c>
+      <c r="D22">
+        <v>244787</v>
+      </c>
+      <c r="E22" s="21">
+        <f t="shared" si="0"/>
+        <v>2.83318287037037E-3</v>
+      </c>
+      <c r="F22">
+        <v>8250</v>
+      </c>
+      <c r="G22">
+        <v>15496</v>
+      </c>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>64</v>
+      </c>
+      <c r="D23">
+        <v>279875</v>
+      </c>
+      <c r="E23" s="21">
+        <f t="shared" si="0"/>
+        <v>3.2392939814814815E-3</v>
+      </c>
+      <c r="F23">
+        <v>8699</v>
+      </c>
+      <c r="G23">
+        <v>17421</v>
+      </c>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>65</v>
+      </c>
+      <c r="D24">
+        <v>282665</v>
+      </c>
+      <c r="E24" s="21">
+        <f t="shared" si="0"/>
+        <v>3.271585648148148E-3</v>
+      </c>
+      <c r="F24">
+        <v>8807</v>
+      </c>
+      <c r="G24">
+        <v>17682</v>
+      </c>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B4">
-        <v>1195</v>
-      </c>
-      <c r="C4">
-        <v>164</v>
-      </c>
-      <c r="D4">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="4">
+        <v>66</v>
+      </c>
+      <c r="D25" s="10">
+        <v>809061</v>
+      </c>
+      <c r="E25" s="20">
+        <f t="shared" si="0"/>
+        <v>9.364131944444444E-3</v>
+      </c>
+      <c r="F25" s="4">
+        <v>18402</v>
+      </c>
+      <c r="G25" s="4">
+        <v>212413</v>
+      </c>
+      <c r="H25" s="14"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="4">
+        <v>66</v>
+      </c>
+      <c r="D26" s="10">
+        <v>595174</v>
+      </c>
+      <c r="E26" s="20">
+        <f t="shared" si="0"/>
+        <v>6.8885879629629635E-3</v>
+      </c>
+      <c r="F26" s="4">
+        <v>12560</v>
+      </c>
+      <c r="G26" s="4">
+        <v>165984</v>
+      </c>
+      <c r="H26" s="14"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="4">
+        <v>66</v>
+      </c>
+      <c r="D27" s="10">
+        <v>666395</v>
+      </c>
+      <c r="E27" s="20">
+        <f t="shared" si="0"/>
+        <v>7.7129050925925924E-3</v>
+      </c>
+      <c r="F27" s="4">
+        <v>15277</v>
+      </c>
+      <c r="G27" s="4">
+        <v>138154</v>
+      </c>
+      <c r="H27" s="14"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="4">
+        <v>66</v>
+      </c>
+      <c r="D28" s="10">
+        <v>1930064</v>
+      </c>
+      <c r="E28" s="20">
+        <f t="shared" si="0"/>
+        <v>2.2338703703703704E-2</v>
+      </c>
+      <c r="F28" s="4">
+        <v>18844</v>
+      </c>
+      <c r="G28" s="4">
+        <v>1341610</v>
+      </c>
+      <c r="H28" s="14"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="13">
+        <v>66</v>
+      </c>
+      <c r="D29" s="14">
+        <v>317918</v>
+      </c>
+      <c r="E29" s="21">
+        <f t="shared" si="0"/>
+        <v>3.6796064814814816E-3</v>
+      </c>
+      <c r="F29" s="13">
+        <v>9113</v>
+      </c>
+      <c r="G29" s="13">
+        <v>18467</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B5">
-        <v>5869</v>
-      </c>
-      <c r="C5">
-        <v>1104</v>
-      </c>
-      <c r="D5">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="B30" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="13">
+        <v>67</v>
+      </c>
+      <c r="D30" s="14">
+        <v>509197</v>
+      </c>
+      <c r="E30" s="21">
+        <f t="shared" si="0"/>
+        <v>5.8934837962962968E-3</v>
+      </c>
+      <c r="F30" s="13">
+        <v>13392</v>
+      </c>
+      <c r="G30" s="13">
+        <v>35294</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="13">
+        <v>68</v>
+      </c>
+      <c r="D31" s="14">
+        <v>664614</v>
+      </c>
+      <c r="E31" s="21">
+        <f t="shared" si="0"/>
+        <v>7.6922916666666667E-3</v>
+      </c>
+      <c r="F31" s="13">
+        <v>15908</v>
+      </c>
+      <c r="G31" s="13">
+        <v>55980</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="13">
+        <v>69</v>
+      </c>
+      <c r="D32" s="14">
+        <v>711559</v>
+      </c>
+      <c r="E32" s="21">
+        <f t="shared" si="0"/>
+        <v>8.235636574074074E-3</v>
+      </c>
+      <c r="F32" s="13">
+        <v>16609</v>
+      </c>
+      <c r="G32" s="13">
+        <v>59892</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="13">
+        <v>70</v>
+      </c>
+      <c r="D33" s="14">
+        <v>743164</v>
+      </c>
+      <c r="E33" s="21">
+        <f t="shared" si="0"/>
+        <v>8.6014351851851859E-3</v>
+      </c>
+      <c r="F33" s="13">
+        <v>17271</v>
+      </c>
+      <c r="G33" s="13">
+        <v>64117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="4">
+        <v>71</v>
+      </c>
+      <c r="D34" s="10">
+        <v>1162769</v>
+      </c>
+      <c r="E34" s="20">
+        <f t="shared" si="0"/>
+        <v>1.3457974537037037E-2</v>
+      </c>
+      <c r="F34" s="4">
+        <v>22690</v>
+      </c>
+      <c r="G34" s="4">
+        <v>207746</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B6">
-        <v>11469</v>
-      </c>
-      <c r="C6">
-        <v>1548</v>
-      </c>
-      <c r="D6">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="B35" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="4">
+        <v>71</v>
+      </c>
+      <c r="D35" s="10">
+        <v>1435281</v>
+      </c>
+      <c r="E35" s="20">
+        <f t="shared" si="0"/>
+        <v>1.661204861111111E-2</v>
+      </c>
+      <c r="F35" s="4">
+        <v>25294</v>
+      </c>
+      <c r="G35" s="4">
+        <v>349558</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B7">
-        <v>18602</v>
-      </c>
-      <c r="C7">
-        <v>1780</v>
-      </c>
-      <c r="D7">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="B36" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="13">
+        <v>71</v>
+      </c>
+      <c r="D36" s="14">
+        <v>1109696</v>
+      </c>
+      <c r="E36" s="21">
+        <f t="shared" si="0"/>
+        <v>1.2843703703703704E-2</v>
+      </c>
+      <c r="F36" s="13">
+        <v>21825</v>
+      </c>
+      <c r="G36" s="13">
+        <v>155955</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="13">
+        <v>72</v>
+      </c>
+      <c r="D37" s="14">
+        <v>1393977</v>
+      </c>
+      <c r="E37" s="21">
+        <f>D37/3600000/24</f>
+        <v>1.6133993055555556E-2</v>
+      </c>
+      <c r="F37" s="13">
+        <v>24691</v>
+      </c>
+      <c r="G37" s="13">
+        <v>249984</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="4">
+        <v>73</v>
+      </c>
+      <c r="D38" s="4">
+        <v>2505126</v>
+      </c>
+      <c r="E38" s="20">
+        <f>D38/3600000/24</f>
+        <v>2.8994513888888889E-2</v>
+      </c>
+      <c r="F38" s="4">
+        <v>38461</v>
+      </c>
+      <c r="G38" s="4">
+        <v>700271</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="13">
+        <v>73</v>
+      </c>
+      <c r="D39" s="13">
+        <v>1614447</v>
+      </c>
+      <c r="E39" s="21">
+        <f t="shared" ref="E39:E46" si="1">D39/3600000/24</f>
+        <v>1.8685729166666668E-2</v>
+      </c>
+      <c r="F39" s="13">
+        <v>26982</v>
+      </c>
+      <c r="G39" s="13">
+        <v>325120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="13">
+        <v>74</v>
+      </c>
+      <c r="D40">
+        <v>1940835</v>
+      </c>
+      <c r="E40" s="21">
+        <f t="shared" si="1"/>
+        <v>2.2463368055555558E-2</v>
+      </c>
+      <c r="F40" s="13">
+        <v>29031</v>
+      </c>
+      <c r="G40" s="13">
+        <v>411064</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B8">
-        <v>30098</v>
-      </c>
-      <c r="C8">
-        <v>2084</v>
-      </c>
-      <c r="D8">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="B41" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="13">
+        <v>75</v>
+      </c>
+      <c r="D41">
+        <v>2114103</v>
+      </c>
+      <c r="E41" s="21">
+        <f t="shared" si="1"/>
+        <v>2.4468784722222223E-2</v>
+      </c>
+      <c r="F41" s="13">
+        <v>31080</v>
+      </c>
+      <c r="G41" s="13">
+        <v>491724</v>
+      </c>
+      <c r="H41" s="21"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B9">
-        <v>32362</v>
-      </c>
-      <c r="C9">
-        <v>2150</v>
-      </c>
-      <c r="D9">
-        <v>1349</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="B42" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="13">
+        <v>76</v>
+      </c>
+      <c r="D42">
+        <v>2364937</v>
+      </c>
+      <c r="E42" s="21">
+        <f t="shared" si="1"/>
+        <v>2.7371956018518519E-2</v>
+      </c>
+      <c r="F42" s="13">
+        <v>33129</v>
+      </c>
+      <c r="G42" s="13">
+        <v>611868</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B10">
-        <v>37169</v>
-      </c>
-      <c r="C10">
-        <v>2290</v>
-      </c>
-      <c r="D10">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="B43" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="13">
+        <v>77</v>
+      </c>
+      <c r="D43">
+        <v>2555695</v>
+      </c>
+      <c r="E43" s="21">
+        <f t="shared" si="1"/>
+        <v>2.9579803240740738E-2</v>
+      </c>
+      <c r="F43" s="13">
+        <v>33899</v>
+      </c>
+      <c r="G43" s="13">
+        <v>626432</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B11">
-        <v>39038</v>
-      </c>
-      <c r="C11">
-        <v>2348</v>
-      </c>
-      <c r="D11">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="B44" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="4">
+        <v>78</v>
+      </c>
+      <c r="D44" s="10">
+        <v>3305786</v>
+      </c>
+      <c r="E44" s="20">
+        <f t="shared" si="1"/>
+        <v>3.8261412037037035E-2</v>
+      </c>
+      <c r="F44" s="4">
+        <v>38749</v>
+      </c>
+      <c r="G44" s="4">
+        <v>1002787</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B12">
-        <v>43830</v>
-      </c>
-      <c r="C12">
-        <v>2416</v>
-      </c>
-      <c r="D12">
-        <v>1138</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>55</v>
-      </c>
-      <c r="B13">
-        <v>47562</v>
-      </c>
-      <c r="C13">
-        <v>2556</v>
-      </c>
-      <c r="D13">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>56</v>
-      </c>
-      <c r="B14">
-        <v>89156</v>
-      </c>
-      <c r="C14">
-        <v>4688</v>
-      </c>
-      <c r="D14">
-        <v>2851</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="B45" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="13">
+        <v>78</v>
+      </c>
+      <c r="D45" s="9"/>
+      <c r="E45" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B15">
-        <v>135472</v>
-      </c>
-      <c r="C15">
-        <v>6606</v>
-      </c>
-      <c r="D15">
-        <v>8143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>58</v>
-      </c>
-      <c r="B16">
-        <v>163843</v>
-      </c>
-      <c r="C16">
-        <v>7296</v>
-      </c>
-      <c r="D16">
-        <v>12443</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>59</v>
-      </c>
-      <c r="B17">
-        <v>198760</v>
-      </c>
-      <c r="C17">
-        <v>8212</v>
-      </c>
-      <c r="D17">
-        <v>14855</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>60</v>
-      </c>
-      <c r="B18">
-        <v>233032</v>
-      </c>
-      <c r="C18">
-        <v>8802</v>
-      </c>
-      <c r="D18">
-        <v>17259</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
-        <v>242919</v>
-      </c>
-      <c r="C23">
-        <v>9974</v>
-      </c>
-      <c r="D23">
-        <v>81722</v>
-      </c>
+      <c r="C46" s="16">
+        <v>82</v>
+      </c>
+      <c r="D46" s="17">
+        <v>15776143.311657</v>
+      </c>
+      <c r="E46" s="22">
+        <f t="shared" si="1"/>
+        <v>0.1825942512923264</v>
+      </c>
+      <c r="F46" s="16">
+        <v>89411</v>
+      </c>
+      <c r="G46" s="16">
+        <v>9528224</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Preprocessing/Analyse algorithm fully working. GUI improved to display plot points and cancel button/timer
</commit_message>
<xml_diff>
--- a/ProcessingTimeExtrapolation.xlsx
+++ b/ProcessingTimeExtrapolation.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
-    <sheet name="Forest1 Processing" sheetId="1" r:id="rId2"/>
+    <sheet name="Chart Manual" sheetId="2" r:id="rId1"/>
+    <sheet name="Forest1 Processing Manual" sheetId="3" r:id="rId2"/>
+    <sheet name="Chart Auto" sheetId="5" r:id="rId3"/>
+    <sheet name="Forest1 Processing Automated" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="74">
   <si>
     <t>No Species</t>
   </si>
@@ -202,7 +205,46 @@
     <t>54,57,58,69,70,71,72,78,79,82</t>
   </si>
   <si>
-    <t>54,57,58,69,70,71,72,78,79,82,88</t>
+    <t>excel</t>
+  </si>
+  <si>
+    <t>java</t>
+  </si>
+  <si>
+    <t>54,58</t>
+  </si>
+  <si>
+    <t>54,58,60</t>
+  </si>
+  <si>
+    <t>54,58,60,69</t>
+  </si>
+  <si>
+    <t>54,58,60,69,70</t>
+  </si>
+  <si>
+    <t>54,58,60,69,70,71</t>
+  </si>
+  <si>
+    <t>54,58,60,69,70,71,72</t>
+  </si>
+  <si>
+    <t>54,58,60,69,70,71,72,78</t>
+  </si>
+  <si>
+    <t>54,58,60,69,70,71,72,78,79</t>
+  </si>
+  <si>
+    <t>54,58,60,69,70,71,72,78,79,82</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Error Margin</t>
+  </si>
+  <si>
+    <t>Additional Test</t>
   </si>
 </sst>
 </file>
@@ -210,7 +252,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="hh:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -221,7 +263,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,6 +282,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -253,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -267,7 +315,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -275,16 +322,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,7 +520,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Forest1 Processing'!$C$2:$C$45</c:f>
+              <c:f>'Forest1 Processing Manual'!$C$2:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
@@ -599,14 +654,14 @@
                   <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>78</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Forest1 Processing'!$D$2:$D$45</c:f>
+              <c:f>'Forest1 Processing Manual'!$D$2:$D$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
@@ -738,6 +793,9 @@
                 </c:pt>
                 <c:pt idx="42" formatCode="0">
                   <c:v>3305786</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="0">
+                  <c:v>4112484</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -809,7 +867,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Forest1 Processing'!$C$2:$C$45</c:f>
+              <c:f>'Forest1 Processing Manual'!$C$2:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
@@ -943,14 +1001,14 @@
                   <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>78</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Forest1 Processing'!$G$2:$G$45</c:f>
+              <c:f>'Forest1 Processing Manual'!$G$2:$G$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
@@ -1082,6 +1140,9 @@
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>1002787</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1423967</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1345,6 +1406,7 @@
         <c:axId val="413704400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1800000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1445,7 +1507,6 @@
         <c:crossAx val="490884776"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1500000"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="490884776"/>
@@ -1543,7 +1604,611 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Forest1 Processing Automated'!$C$2:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>79</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Forest1 Processing Automated'!$D$2:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>4503</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4376</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4708</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4827</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128225</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5130</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5225</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12440</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25661</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32198</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23507</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30272</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>37470</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44229</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>57789</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>79732</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>96510</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>99013</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>461014</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>323497</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>600242</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2039310</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>102443</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>197416</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>478511</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>577750</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>646910</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1336053</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1819359</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1099992</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1477043</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3875593</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1815057</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1815360</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3221309</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3787043</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3994613</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3971849</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5258059</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-11F9-4EF6-A9AE-59FF068E200F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="556485632"/>
+        <c:axId val="556488256"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="556485632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="556488256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="556488256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="556485632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2099,6 +2764,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
@@ -2110,7 +3291,45 @@
 </chartsheet>
 </file>
 
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9290911" cy="6045953"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -2134,6 +3353,49 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>599106</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>18362</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="66675" y="8039100"/>
+          <a:ext cx="7752381" cy="5504762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2400,11 +3662,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
+      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2418,6 +3680,1155 @@
     <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>1195</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2">
+        <v>164</v>
+      </c>
+      <c r="G2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>5869</v>
+      </c>
+      <c r="E3" s="20">
+        <f t="shared" ref="E3:E36" si="0">D3/3600000/24</f>
+        <v>6.7928240740740742E-5</v>
+      </c>
+      <c r="F3">
+        <v>1104</v>
+      </c>
+      <c r="G3">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <v>11469</v>
+      </c>
+      <c r="E4" s="20">
+        <f t="shared" si="0"/>
+        <v>1.3274305555555557E-4</v>
+      </c>
+      <c r="F4">
+        <v>1548</v>
+      </c>
+      <c r="G4">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>45</v>
+      </c>
+      <c r="D5">
+        <v>18602</v>
+      </c>
+      <c r="E5" s="20">
+        <f t="shared" si="0"/>
+        <v>2.1530092592592594E-4</v>
+      </c>
+      <c r="F5">
+        <v>1780</v>
+      </c>
+      <c r="G5">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>30098</v>
+      </c>
+      <c r="E6" s="20">
+        <f t="shared" si="0"/>
+        <v>3.4835648148148144E-4</v>
+      </c>
+      <c r="F6">
+        <v>2084</v>
+      </c>
+      <c r="G6">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>51</v>
+      </c>
+      <c r="D7">
+        <v>32362</v>
+      </c>
+      <c r="E7" s="20">
+        <f t="shared" si="0"/>
+        <v>3.7456018518518518E-4</v>
+      </c>
+      <c r="F7">
+        <v>2150</v>
+      </c>
+      <c r="G7">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>52</v>
+      </c>
+      <c r="D8">
+        <v>37169</v>
+      </c>
+      <c r="E8" s="20">
+        <f t="shared" si="0"/>
+        <v>4.3019675925925929E-4</v>
+      </c>
+      <c r="F8">
+        <v>2290</v>
+      </c>
+      <c r="G8">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>53</v>
+      </c>
+      <c r="D9">
+        <v>39038</v>
+      </c>
+      <c r="E9" s="20">
+        <f t="shared" si="0"/>
+        <v>4.5182870370370369E-4</v>
+      </c>
+      <c r="F9">
+        <v>2348</v>
+      </c>
+      <c r="G9">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4">
+        <v>54</v>
+      </c>
+      <c r="D10" s="4">
+        <v>242919</v>
+      </c>
+      <c r="E10" s="19">
+        <f t="shared" si="0"/>
+        <v>2.8115624999999998E-3</v>
+      </c>
+      <c r="F10" s="4">
+        <v>9974</v>
+      </c>
+      <c r="G10" s="4">
+        <v>81722</v>
+      </c>
+      <c r="H10" s="12"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>54</v>
+      </c>
+      <c r="C11">
+        <v>54</v>
+      </c>
+      <c r="D11">
+        <v>43830</v>
+      </c>
+      <c r="E11" s="20">
+        <f t="shared" si="0"/>
+        <v>5.0729166666666663E-4</v>
+      </c>
+      <c r="F11">
+        <v>2416</v>
+      </c>
+      <c r="G11">
+        <v>1138</v>
+      </c>
+      <c r="H11" s="12"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>54</v>
+      </c>
+      <c r="C12">
+        <v>55</v>
+      </c>
+      <c r="D12">
+        <v>47562</v>
+      </c>
+      <c r="E12" s="20">
+        <f t="shared" si="0"/>
+        <v>5.5048611111111108E-4</v>
+      </c>
+      <c r="F12">
+        <v>2556</v>
+      </c>
+      <c r="G12">
+        <v>1107</v>
+      </c>
+      <c r="H12" s="12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4">
+        <v>54</v>
+      </c>
+      <c r="C13" s="4">
+        <v>56</v>
+      </c>
+      <c r="D13" s="4">
+        <v>89156</v>
+      </c>
+      <c r="E13" s="19">
+        <f t="shared" si="0"/>
+        <v>1.0318981481481481E-3</v>
+      </c>
+      <c r="F13" s="4">
+        <v>4688</v>
+      </c>
+      <c r="G13" s="4">
+        <v>2851</v>
+      </c>
+      <c r="H13" s="12"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="4">
+        <v>56</v>
+      </c>
+      <c r="D14" s="4">
+        <v>82084</v>
+      </c>
+      <c r="E14" s="19">
+        <f t="shared" si="0"/>
+        <v>9.5004629629629638E-4</v>
+      </c>
+      <c r="F14" s="4">
+        <v>4056</v>
+      </c>
+      <c r="G14" s="4">
+        <v>3492</v>
+      </c>
+      <c r="H14" s="12"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>56</v>
+      </c>
+      <c r="D15">
+        <v>55626</v>
+      </c>
+      <c r="E15" s="20">
+        <f t="shared" si="0"/>
+        <v>6.4381944444444447E-4</v>
+      </c>
+      <c r="F15">
+        <v>2790</v>
+      </c>
+      <c r="G15">
+        <v>1549</v>
+      </c>
+      <c r="H15" s="12"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>57</v>
+      </c>
+      <c r="D16">
+        <v>73297</v>
+      </c>
+      <c r="E16" s="20">
+        <f t="shared" si="0"/>
+        <v>8.4834490740740747E-4</v>
+      </c>
+      <c r="F16">
+        <v>3328</v>
+      </c>
+      <c r="G16">
+        <v>4091</v>
+      </c>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <v>58</v>
+      </c>
+      <c r="D17">
+        <v>79340</v>
+      </c>
+      <c r="E17" s="20">
+        <f t="shared" si="0"/>
+        <v>9.1828703703703701E-4</v>
+      </c>
+      <c r="F17">
+        <v>3554</v>
+      </c>
+      <c r="G17">
+        <v>2924</v>
+      </c>
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>59</v>
+      </c>
+      <c r="D18">
+        <v>96783</v>
+      </c>
+      <c r="E18" s="20">
+        <f t="shared" si="0"/>
+        <v>1.1201736111111111E-3</v>
+      </c>
+      <c r="F18">
+        <v>4040</v>
+      </c>
+      <c r="G18">
+        <v>4344</v>
+      </c>
+      <c r="H18" s="12"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19">
+        <v>60</v>
+      </c>
+      <c r="D19">
+        <v>120869</v>
+      </c>
+      <c r="E19" s="20">
+        <f t="shared" si="0"/>
+        <v>1.3989467592592593E-3</v>
+      </c>
+      <c r="F19">
+        <v>4866</v>
+      </c>
+      <c r="G19">
+        <v>5882</v>
+      </c>
+      <c r="H19" s="12"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>61</v>
+      </c>
+      <c r="D20">
+        <v>139989</v>
+      </c>
+      <c r="E20" s="20">
+        <f t="shared" si="0"/>
+        <v>1.6202430555555555E-3</v>
+      </c>
+      <c r="F20">
+        <v>5004</v>
+      </c>
+      <c r="G20">
+        <v>5875</v>
+      </c>
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>62</v>
+      </c>
+      <c r="D21">
+        <v>180415</v>
+      </c>
+      <c r="E21" s="20">
+        <f t="shared" si="0"/>
+        <v>2.0881365740740743E-3</v>
+      </c>
+      <c r="F21">
+        <v>6404</v>
+      </c>
+      <c r="G21">
+        <v>9828</v>
+      </c>
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22">
+        <v>63</v>
+      </c>
+      <c r="D22">
+        <v>244787</v>
+      </c>
+      <c r="E22" s="20">
+        <f t="shared" si="0"/>
+        <v>2.83318287037037E-3</v>
+      </c>
+      <c r="F22">
+        <v>8250</v>
+      </c>
+      <c r="G22">
+        <v>15496</v>
+      </c>
+      <c r="H22" s="12"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>64</v>
+      </c>
+      <c r="D23">
+        <v>279875</v>
+      </c>
+      <c r="E23" s="20">
+        <f t="shared" si="0"/>
+        <v>3.2392939814814815E-3</v>
+      </c>
+      <c r="F23">
+        <v>8699</v>
+      </c>
+      <c r="G23">
+        <v>17421</v>
+      </c>
+      <c r="H23" s="12"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>65</v>
+      </c>
+      <c r="D24">
+        <v>282665</v>
+      </c>
+      <c r="E24" s="20">
+        <f t="shared" si="0"/>
+        <v>3.271585648148148E-3</v>
+      </c>
+      <c r="F24">
+        <v>8807</v>
+      </c>
+      <c r="G24">
+        <v>17682</v>
+      </c>
+      <c r="H24" s="12"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="4">
+        <v>66</v>
+      </c>
+      <c r="D25" s="9">
+        <v>809061</v>
+      </c>
+      <c r="E25" s="19">
+        <f t="shared" si="0"/>
+        <v>9.364131944444444E-3</v>
+      </c>
+      <c r="F25" s="4">
+        <v>18402</v>
+      </c>
+      <c r="G25" s="4">
+        <v>212413</v>
+      </c>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="4">
+        <v>66</v>
+      </c>
+      <c r="D26" s="9">
+        <v>595174</v>
+      </c>
+      <c r="E26" s="19">
+        <f t="shared" si="0"/>
+        <v>6.8885879629629635E-3</v>
+      </c>
+      <c r="F26" s="4">
+        <v>12560</v>
+      </c>
+      <c r="G26" s="4">
+        <v>165984</v>
+      </c>
+      <c r="H26" s="13"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="4">
+        <v>66</v>
+      </c>
+      <c r="D27" s="9">
+        <v>666395</v>
+      </c>
+      <c r="E27" s="19">
+        <f t="shared" si="0"/>
+        <v>7.7129050925925924E-3</v>
+      </c>
+      <c r="F27" s="4">
+        <v>15277</v>
+      </c>
+      <c r="G27" s="4">
+        <v>138154</v>
+      </c>
+      <c r="H27" s="13"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="4">
+        <v>66</v>
+      </c>
+      <c r="D28" s="9">
+        <v>1930064</v>
+      </c>
+      <c r="E28" s="19">
+        <f t="shared" si="0"/>
+        <v>2.2338703703703704E-2</v>
+      </c>
+      <c r="F28" s="4">
+        <v>18844</v>
+      </c>
+      <c r="G28" s="4">
+        <v>1341610</v>
+      </c>
+      <c r="H28" s="13"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="12">
+        <v>66</v>
+      </c>
+      <c r="D29" s="13">
+        <v>317918</v>
+      </c>
+      <c r="E29" s="20">
+        <f t="shared" si="0"/>
+        <v>3.6796064814814816E-3</v>
+      </c>
+      <c r="F29" s="12">
+        <v>9113</v>
+      </c>
+      <c r="G29" s="12">
+        <v>18467</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="12">
+        <v>67</v>
+      </c>
+      <c r="D30" s="13">
+        <v>509197</v>
+      </c>
+      <c r="E30" s="20">
+        <f t="shared" si="0"/>
+        <v>5.8934837962962968E-3</v>
+      </c>
+      <c r="F30" s="12">
+        <v>13392</v>
+      </c>
+      <c r="G30" s="12">
+        <v>35294</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="12">
+        <v>68</v>
+      </c>
+      <c r="D31" s="13">
+        <v>664614</v>
+      </c>
+      <c r="E31" s="20">
+        <f t="shared" si="0"/>
+        <v>7.6922916666666667E-3</v>
+      </c>
+      <c r="F31" s="12">
+        <v>15908</v>
+      </c>
+      <c r="G31" s="12">
+        <v>55980</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="12">
+        <v>69</v>
+      </c>
+      <c r="D32" s="13">
+        <v>711559</v>
+      </c>
+      <c r="E32" s="20">
+        <f t="shared" si="0"/>
+        <v>8.235636574074074E-3</v>
+      </c>
+      <c r="F32" s="12">
+        <v>16609</v>
+      </c>
+      <c r="G32" s="12">
+        <v>59892</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="12">
+        <v>70</v>
+      </c>
+      <c r="D33" s="13">
+        <v>743164</v>
+      </c>
+      <c r="E33" s="20">
+        <f t="shared" si="0"/>
+        <v>8.6014351851851859E-3</v>
+      </c>
+      <c r="F33" s="12">
+        <v>17271</v>
+      </c>
+      <c r="G33" s="12">
+        <v>64117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="4">
+        <v>71</v>
+      </c>
+      <c r="D34" s="9">
+        <v>1162769</v>
+      </c>
+      <c r="E34" s="19">
+        <f t="shared" si="0"/>
+        <v>1.3457974537037037E-2</v>
+      </c>
+      <c r="F34" s="4">
+        <v>22690</v>
+      </c>
+      <c r="G34" s="4">
+        <v>207746</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="4">
+        <v>71</v>
+      </c>
+      <c r="D35" s="9">
+        <v>1435281</v>
+      </c>
+      <c r="E35" s="19">
+        <f t="shared" si="0"/>
+        <v>1.661204861111111E-2</v>
+      </c>
+      <c r="F35" s="4">
+        <v>25294</v>
+      </c>
+      <c r="G35" s="4">
+        <v>349558</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="12">
+        <v>71</v>
+      </c>
+      <c r="D36" s="13">
+        <v>1109696</v>
+      </c>
+      <c r="E36" s="20">
+        <f t="shared" si="0"/>
+        <v>1.2843703703703704E-2</v>
+      </c>
+      <c r="F36" s="12">
+        <v>21825</v>
+      </c>
+      <c r="G36" s="12">
+        <v>155955</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="12">
+        <v>72</v>
+      </c>
+      <c r="D37" s="13">
+        <v>1393977</v>
+      </c>
+      <c r="E37" s="20">
+        <f>D37/3600000/24</f>
+        <v>1.6133993055555556E-2</v>
+      </c>
+      <c r="F37" s="12">
+        <v>24691</v>
+      </c>
+      <c r="G37" s="12">
+        <v>249984</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="4">
+        <v>73</v>
+      </c>
+      <c r="D38" s="4">
+        <v>2505126</v>
+      </c>
+      <c r="E38" s="19">
+        <f>D38/3600000/24</f>
+        <v>2.8994513888888889E-2</v>
+      </c>
+      <c r="F38" s="4">
+        <v>38461</v>
+      </c>
+      <c r="G38" s="4">
+        <v>700271</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="12">
+        <v>73</v>
+      </c>
+      <c r="D39" s="12">
+        <v>1614447</v>
+      </c>
+      <c r="E39" s="20">
+        <f t="shared" ref="E39:E48" si="1">D39/3600000/24</f>
+        <v>1.8685729166666668E-2</v>
+      </c>
+      <c r="F39" s="12">
+        <v>26982</v>
+      </c>
+      <c r="G39" s="12">
+        <v>325120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="12">
+        <v>74</v>
+      </c>
+      <c r="D40">
+        <v>1940835</v>
+      </c>
+      <c r="E40" s="20">
+        <f t="shared" si="1"/>
+        <v>2.2463368055555558E-2</v>
+      </c>
+      <c r="F40" s="12">
+        <v>29031</v>
+      </c>
+      <c r="G40" s="12">
+        <v>411064</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="12">
+        <v>75</v>
+      </c>
+      <c r="D41">
+        <v>2114103</v>
+      </c>
+      <c r="E41" s="20">
+        <f t="shared" si="1"/>
+        <v>2.4468784722222223E-2</v>
+      </c>
+      <c r="F41" s="12">
+        <v>31080</v>
+      </c>
+      <c r="G41" s="12">
+        <v>491724</v>
+      </c>
+      <c r="H41" s="20"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="12">
+        <v>76</v>
+      </c>
+      <c r="D42">
+        <v>2364937</v>
+      </c>
+      <c r="E42" s="20">
+        <f t="shared" si="1"/>
+        <v>2.7371956018518519E-2</v>
+      </c>
+      <c r="F42" s="12">
+        <v>33129</v>
+      </c>
+      <c r="G42" s="12">
+        <v>611868</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="12">
+        <v>77</v>
+      </c>
+      <c r="D43">
+        <v>2555695</v>
+      </c>
+      <c r="E43" s="20">
+        <f t="shared" si="1"/>
+        <v>2.9579803240740738E-2</v>
+      </c>
+      <c r="F43" s="12">
+        <v>33899</v>
+      </c>
+      <c r="G43" s="12">
+        <v>626432</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="12">
+        <v>78</v>
+      </c>
+      <c r="D44" s="13">
+        <v>3305786</v>
+      </c>
+      <c r="E44" s="20">
+        <f t="shared" si="1"/>
+        <v>3.8261412037037035E-2</v>
+      </c>
+      <c r="F44" s="12">
+        <v>38749</v>
+      </c>
+      <c r="G44" s="12">
+        <v>1002787</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="12">
+        <v>79</v>
+      </c>
+      <c r="D45" s="13">
+        <v>4112484</v>
+      </c>
+      <c r="E45" s="20">
+        <f t="shared" si="1"/>
+        <v>4.7598194444444443E-2</v>
+      </c>
+      <c r="F45" s="12">
+        <v>43556</v>
+      </c>
+      <c r="G45" s="12">
+        <v>1423967</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E46" s="14">
+        <f>SUM(E3:E45)</f>
+        <v>0.40273247685185182</v>
+      </c>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="15">
+        <v>82</v>
+      </c>
+      <c r="D48" s="16">
+        <v>15776143.311657</v>
+      </c>
+      <c r="E48" s="21">
+        <f t="shared" si="1"/>
+        <v>0.1825942512923264</v>
+      </c>
+      <c r="F48" s="15">
+        <v>89411</v>
+      </c>
+      <c r="G48" s="15">
+        <v>9528224</v>
+      </c>
+      <c r="H48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D49" s="8"/>
+      <c r="E49" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L50" sqref="L50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
@@ -2442,1111 +4853,1247 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
+      <c r="A2" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D2">
-        <v>1195</v>
-      </c>
-      <c r="E2" s="15"/>
+        <v>4503</v>
+      </c>
+      <c r="E2" s="20">
+        <f t="shared" ref="E2:E41" si="0">D2/3600000/24</f>
+        <v>5.2118055555555556E-5</v>
+      </c>
       <c r="F2">
-        <v>164</v>
+        <v>2016</v>
       </c>
       <c r="G2">
-        <v>117</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C3">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="D3">
-        <v>5869</v>
-      </c>
-      <c r="E3" s="21">
-        <f t="shared" ref="E3:E36" si="0">D3/3600000/24</f>
-        <v>6.7928240740740742E-5</v>
+        <v>4376</v>
+      </c>
+      <c r="E3" s="20">
+        <f t="shared" si="0"/>
+        <v>5.0648148148148155E-5</v>
       </c>
       <c r="F3">
-        <v>1104</v>
+        <v>2078</v>
       </c>
       <c r="G3">
-        <v>392</v>
+        <v>1191</v>
+      </c>
+      <c r="I3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D4">
-        <v>11469</v>
-      </c>
-      <c r="E4" s="21">
-        <f t="shared" si="0"/>
-        <v>1.3274305555555557E-4</v>
+        <v>4708</v>
+      </c>
+      <c r="E4" s="20">
+        <f t="shared" si="0"/>
+        <v>5.449074074074074E-5</v>
       </c>
       <c r="F4">
-        <v>1548</v>
+        <v>2214</v>
       </c>
       <c r="G4">
-        <v>612</v>
+        <v>1434</v>
+      </c>
+      <c r="I4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C5">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D5">
-        <v>18602</v>
-      </c>
-      <c r="E5" s="21">
-        <f t="shared" si="0"/>
-        <v>2.1530092592592594E-4</v>
+        <v>4827</v>
+      </c>
+      <c r="E5" s="20">
+        <f t="shared" si="0"/>
+        <v>5.5868055555555559E-5</v>
       </c>
       <c r="F5">
-        <v>1780</v>
+        <v>2272</v>
       </c>
       <c r="G5">
-        <v>725</v>
+        <v>1372</v>
+      </c>
+      <c r="I5" s="8">
+        <f>D5/(1079 * EXP(0.0282*C5))</f>
+        <v>1.0035969238625546</v>
+      </c>
+      <c r="J5" s="8">
+        <v>1.0595570000000001</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>50</v>
-      </c>
-      <c r="D6">
-        <v>30098</v>
-      </c>
-      <c r="E6" s="21">
-        <f t="shared" si="0"/>
-        <v>3.4835648148148144E-4</v>
-      </c>
-      <c r="F6">
-        <v>2084</v>
-      </c>
-      <c r="G6">
-        <v>906</v>
+      <c r="A6" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23">
+        <v>54</v>
+      </c>
+      <c r="D6" s="23">
+        <v>128225</v>
+      </c>
+      <c r="E6" s="24">
+        <f t="shared" si="0"/>
+        <v>1.4840856481481482E-3</v>
+      </c>
+      <c r="F6" s="23">
+        <v>9312</v>
+      </c>
+      <c r="G6" s="23">
+        <v>114744</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="25">
+        <f>D6/(0.000000000004 * EXP(0.6796*C6))</f>
+        <v>3.698282664108667</v>
+      </c>
+      <c r="J6" s="25">
+        <v>3.6800220000000001</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>54</v>
       </c>
       <c r="C7">
-        <v>51</v>
-      </c>
-      <c r="D7">
-        <v>32362</v>
-      </c>
-      <c r="E7" s="21">
-        <f t="shared" si="0"/>
-        <v>3.7456018518518518E-4</v>
-      </c>
-      <c r="F7">
-        <v>2150</v>
-      </c>
-      <c r="G7">
-        <v>1349</v>
+        <v>54</v>
+      </c>
+      <c r="D7" s="12">
+        <v>5130</v>
+      </c>
+      <c r="E7" s="20">
+        <f t="shared" si="0"/>
+        <v>5.9375E-5</v>
+      </c>
+      <c r="F7" s="12">
+        <v>2340</v>
+      </c>
+      <c r="G7" s="12">
+        <v>1391</v>
+      </c>
+      <c r="I7" s="8">
+        <f>D7/(0.0000008 * EXP(0.4401*C7))</f>
+        <v>0.30608729113694755</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0.30199300000000001</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>54</v>
       </c>
       <c r="C8">
-        <v>52</v>
-      </c>
-      <c r="D8">
-        <v>37169</v>
-      </c>
-      <c r="E8" s="21">
-        <f t="shared" si="0"/>
-        <v>4.3019675925925929E-4</v>
-      </c>
-      <c r="F8">
-        <v>2290</v>
-      </c>
-      <c r="G8">
-        <v>1011</v>
+        <v>55</v>
+      </c>
+      <c r="D8" s="12">
+        <v>5225</v>
+      </c>
+      <c r="E8" s="20">
+        <f t="shared" si="0"/>
+        <v>6.047453703703703E-5</v>
+      </c>
+      <c r="F8" s="12">
+        <v>2480</v>
+      </c>
+      <c r="G8" s="12">
+        <v>1460</v>
+      </c>
+      <c r="I8" s="8">
+        <f>D8/(0.0147 * EXP(0.2497*C8))</f>
+        <v>0.38582084940405598</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0.38574467000000001</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>13</v>
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>54</v>
       </c>
       <c r="C9">
-        <v>53</v>
-      </c>
-      <c r="D9">
-        <v>39038</v>
-      </c>
-      <c r="E9" s="21">
-        <f t="shared" si="0"/>
-        <v>4.5182870370370369E-4</v>
-      </c>
-      <c r="F9">
-        <v>2348</v>
-      </c>
-      <c r="G9">
-        <v>976</v>
+        <v>56</v>
+      </c>
+      <c r="D9" s="12">
+        <v>12440</v>
+      </c>
+      <c r="E9" s="20">
+        <f t="shared" si="0"/>
+        <v>1.4398148148148148E-4</v>
+      </c>
+      <c r="F9" s="12">
+        <v>4612</v>
+      </c>
+      <c r="G9" s="12">
+        <v>5243</v>
+      </c>
+      <c r="I9" s="8">
+        <f>D9/(0.083 * EXP(0.2163*C9))</f>
+        <v>0.82265944377033384</v>
+      </c>
+      <c r="J9" s="8">
+        <v>0.82123365999999998</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4">
+      <c r="A10" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="23">
         <v>54</v>
       </c>
-      <c r="D10" s="4">
-        <v>242919</v>
-      </c>
-      <c r="E10" s="20">
-        <f t="shared" si="0"/>
-        <v>2.8115624999999998E-3</v>
-      </c>
-      <c r="F10" s="4">
-        <v>9974</v>
-      </c>
-      <c r="G10" s="4">
-        <v>81722</v>
-      </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
+      <c r="C10" s="23">
+        <v>57</v>
+      </c>
+      <c r="D10" s="23">
+        <v>25661</v>
+      </c>
+      <c r="E10" s="24">
+        <f t="shared" si="0"/>
+        <v>2.9700231481481483E-4</v>
+      </c>
+      <c r="F10" s="23">
+        <v>6526</v>
+      </c>
+      <c r="G10" s="23">
+        <v>15369</v>
+      </c>
+      <c r="H10" s="23"/>
+      <c r="I10" s="25">
+        <f>D10/(0.0221 * EXP(0.2417*C10))</f>
+        <v>1.2068398862768051</v>
+      </c>
+      <c r="J10" s="25">
+        <v>1.2078285</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
-        <v>54</v>
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="C11">
-        <v>54</v>
-      </c>
-      <c r="D11">
-        <v>43830</v>
-      </c>
-      <c r="E11" s="21">
-        <f t="shared" si="0"/>
-        <v>5.0729166666666663E-4</v>
-      </c>
-      <c r="F11">
-        <v>2416</v>
-      </c>
-      <c r="G11">
-        <v>1138</v>
-      </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
+        <v>57</v>
+      </c>
+      <c r="D11" s="12">
+        <v>18288</v>
+      </c>
+      <c r="E11" s="20">
+        <f t="shared" si="0"/>
+        <v>2.1166666666666667E-4</v>
+      </c>
+      <c r="F11" s="12">
+        <v>5296</v>
+      </c>
+      <c r="G11" s="12">
+        <v>10054</v>
+      </c>
+      <c r="I11" s="8">
+        <f>D11/(0.0349 * EXP(0.2329*C11))</f>
+        <v>0.89939661867057397</v>
+      </c>
+      <c r="J11" s="8">
+        <v>0.89793926000000002</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>54</v>
-      </c>
-      <c r="C12">
-        <v>55</v>
-      </c>
-      <c r="D12">
-        <v>47562</v>
-      </c>
-      <c r="E12" s="21">
-        <f t="shared" si="0"/>
-        <v>5.5048611111111108E-4</v>
-      </c>
-      <c r="F12">
-        <v>2556</v>
-      </c>
-      <c r="G12">
-        <v>1107</v>
-      </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
+      <c r="A12" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="23">
+        <v>58</v>
+      </c>
+      <c r="D12" s="23">
+        <v>32198</v>
+      </c>
+      <c r="E12" s="24">
+        <f t="shared" si="0"/>
+        <v>3.7266203703703702E-4</v>
+      </c>
+      <c r="F12" s="23">
+        <v>6208</v>
+      </c>
+      <c r="G12" s="23">
+        <v>22080</v>
+      </c>
+      <c r="H12" s="23"/>
+      <c r="I12" s="25">
+        <f>D12/(0.0183 * EXP(0.2452*C12))</f>
+        <v>1.1722369388039982</v>
+      </c>
+      <c r="J12" s="25">
+        <v>1.1720268</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="4">
-        <v>54</v>
-      </c>
-      <c r="C13" s="4">
-        <v>56</v>
-      </c>
-      <c r="D13" s="4">
-        <v>89156</v>
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13">
+        <v>58</v>
+      </c>
+      <c r="D13" s="12">
+        <v>23507</v>
       </c>
       <c r="E13" s="20">
         <f t="shared" si="0"/>
-        <v>1.0318981481481481E-3</v>
-      </c>
-      <c r="F13" s="4">
-        <v>4688</v>
-      </c>
-      <c r="G13" s="4">
-        <v>2851</v>
-      </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
+        <v>2.7207175925925928E-4</v>
+      </c>
+      <c r="F13" s="12">
+        <v>5882</v>
+      </c>
+      <c r="G13" s="12">
+        <v>14043</v>
+      </c>
+      <c r="I13" s="8">
+        <f>D13/(0.0259 * EXP(0.2386*C13))</f>
+        <v>0.88671277831720663</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0.88659100000000002</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="4">
-        <v>56</v>
-      </c>
-      <c r="D14" s="4">
-        <v>82084</v>
+      <c r="A14" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="12">
+        <v>59</v>
+      </c>
+      <c r="D14" s="12">
+        <v>30272</v>
       </c>
       <c r="E14" s="20">
         <f t="shared" si="0"/>
-        <v>9.5004629629629638E-4</v>
-      </c>
-      <c r="F14" s="4">
-        <v>4056</v>
-      </c>
-      <c r="G14" s="4">
-        <v>3492</v>
-      </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
+        <v>3.5037037037037041E-4</v>
+      </c>
+      <c r="F14" s="12">
+        <v>6740</v>
+      </c>
+      <c r="G14" s="12">
+        <v>20186</v>
+      </c>
+      <c r="H14" s="12"/>
+      <c r="I14" s="27">
+        <f>D14/(0.0326 * EXP(0.2343*C14))</f>
+        <v>0.92101538560657426</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0.92299399999999998</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15">
-        <v>56</v>
-      </c>
-      <c r="D15">
-        <v>55626</v>
-      </c>
-      <c r="E15" s="21">
-        <f t="shared" si="0"/>
-        <v>6.4381944444444447E-4</v>
-      </c>
-      <c r="F15">
-        <v>2790</v>
-      </c>
-      <c r="G15">
-        <v>1549</v>
-      </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="12">
+        <v>60</v>
+      </c>
+      <c r="D15" s="12">
+        <v>37470</v>
+      </c>
+      <c r="E15" s="20">
+        <f t="shared" si="0"/>
+        <v>4.3368055555555559E-4</v>
+      </c>
+      <c r="F15" s="12">
+        <v>7938</v>
+      </c>
+      <c r="G15" s="12">
+        <v>25513</v>
+      </c>
+      <c r="I15" s="27">
+        <f>D15/(0.0401 * EXP(0.2304*C15))</f>
+        <v>0.92651488870971366</v>
+      </c>
+      <c r="J15" s="8">
+        <v>0.92720789000000003</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16">
-        <v>57</v>
-      </c>
-      <c r="D16">
-        <v>73297</v>
-      </c>
-      <c r="E16" s="21">
-        <f t="shared" si="0"/>
-        <v>8.4834490740740747E-4</v>
-      </c>
-      <c r="F16">
-        <v>3328</v>
-      </c>
-      <c r="G16">
-        <v>4091</v>
-      </c>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
+        <v>25</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="12">
+        <v>61</v>
+      </c>
+      <c r="D16" s="12">
+        <v>44229</v>
+      </c>
+      <c r="E16" s="20">
+        <f t="shared" si="0"/>
+        <v>5.1190972222222219E-4</v>
+      </c>
+      <c r="F16" s="12">
+        <v>8598</v>
+      </c>
+      <c r="G16" s="12">
+        <v>30884</v>
+      </c>
+      <c r="I16" s="27">
+        <f>D16/(0.0521 * EXP(0.2255*C16))</f>
+        <v>0.90142926033925375</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0.90052667900000005</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17">
-        <v>58</v>
-      </c>
-      <c r="D17">
-        <v>79340</v>
-      </c>
-      <c r="E17" s="21">
-        <f t="shared" si="0"/>
-        <v>9.1828703703703701E-4</v>
-      </c>
-      <c r="F17">
-        <v>3554</v>
-      </c>
-      <c r="G17">
-        <v>2924</v>
-      </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
+      <c r="A17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="12">
+        <v>62</v>
+      </c>
+      <c r="D17" s="12">
+        <v>57789</v>
+      </c>
+      <c r="E17" s="20">
+        <f t="shared" si="0"/>
+        <v>6.6885416666666666E-4</v>
+      </c>
+      <c r="F17" s="12">
+        <v>10040</v>
+      </c>
+      <c r="G17" s="12">
+        <v>41864</v>
+      </c>
+      <c r="I17" s="27">
+        <f>D17/(0.0579 * EXP(0.2236*C17))</f>
+        <v>0.95160201747672868</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0.95376260000000002</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18">
-        <v>59</v>
-      </c>
-      <c r="D18">
-        <v>96783</v>
-      </c>
-      <c r="E18" s="21">
-        <f t="shared" si="0"/>
-        <v>1.1201736111111111E-3</v>
-      </c>
-      <c r="F18">
-        <v>4040</v>
-      </c>
-      <c r="G18">
-        <v>4344</v>
-      </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
+        <v>27</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="12">
+        <v>63</v>
+      </c>
+      <c r="D18" s="12">
+        <v>79732</v>
+      </c>
+      <c r="E18" s="20">
+        <f t="shared" si="0"/>
+        <v>9.2282407407407406E-4</v>
+      </c>
+      <c r="F18" s="12">
+        <v>12034</v>
+      </c>
+      <c r="G18" s="12">
+        <v>61432</v>
+      </c>
+      <c r="I18" s="27">
+        <f>D18/(0.0537 * EXP(0.225*C18))</f>
+        <v>1.0364159581998058</v>
+      </c>
+      <c r="J18" s="8">
+        <v>1.0395300000000001</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19">
-        <v>60</v>
-      </c>
-      <c r="D19">
-        <v>120869</v>
-      </c>
-      <c r="E19" s="21">
-        <f t="shared" si="0"/>
-        <v>1.3989467592592593E-3</v>
-      </c>
-      <c r="F19">
-        <v>4866</v>
-      </c>
-      <c r="G19">
-        <v>5882</v>
-      </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
+        <v>28</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="12">
+        <v>64</v>
+      </c>
+      <c r="D19" s="12">
+        <v>96510</v>
+      </c>
+      <c r="E19" s="20">
+        <f t="shared" si="0"/>
+        <v>1.117013888888889E-3</v>
+      </c>
+      <c r="F19" s="12">
+        <v>12962</v>
+      </c>
+      <c r="G19" s="12">
+        <v>77098</v>
+      </c>
+      <c r="I19" s="27">
+        <f>D19/(0.0533 * EXP(0.2251*C19))</f>
+        <v>1.0028248390714889</v>
+      </c>
+      <c r="J19" s="8">
+        <v>1.0036700000000001</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20">
-        <v>61</v>
-      </c>
-      <c r="D20">
-        <v>139989</v>
-      </c>
-      <c r="E20" s="21">
-        <f t="shared" si="0"/>
-        <v>1.6202430555555555E-3</v>
-      </c>
-      <c r="F20">
-        <v>5004</v>
-      </c>
-      <c r="G20">
-        <v>5875</v>
-      </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
+        <v>29</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="12">
+        <v>65</v>
+      </c>
+      <c r="D20" s="12">
+        <v>99013</v>
+      </c>
+      <c r="E20" s="20">
+        <f t="shared" si="0"/>
+        <v>1.1459837962962962E-3</v>
+      </c>
+      <c r="F20" s="12">
+        <v>13060</v>
+      </c>
+      <c r="G20" s="12">
+        <v>77310</v>
+      </c>
+      <c r="I20" s="27">
+        <f>D20/(0.0674 * EXP(0.2208*C20))</f>
+        <v>0.8590885259621327</v>
+      </c>
+      <c r="J20" s="8">
+        <v>0.85840556999999995</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21">
-        <v>62</v>
-      </c>
-      <c r="D21">
-        <v>180415</v>
-      </c>
-      <c r="E21" s="21">
-        <f t="shared" si="0"/>
-        <v>2.0881365740740743E-3</v>
-      </c>
-      <c r="F21">
-        <v>6404</v>
-      </c>
-      <c r="G21">
-        <v>9828</v>
-      </c>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
+      <c r="A21" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="23">
+        <v>66</v>
+      </c>
+      <c r="D21" s="23">
+        <v>461014</v>
+      </c>
+      <c r="E21" s="24">
+        <f t="shared" si="0"/>
+        <v>5.3358101851851856E-3</v>
+      </c>
+      <c r="F21" s="23">
+        <v>21628</v>
+      </c>
+      <c r="G21" s="23">
+        <v>428326</v>
+      </c>
+      <c r="H21" s="23"/>
+      <c r="I21" s="25">
+        <f>D21/(0.0193 * EXP(0.2435*C21))</f>
+        <v>2.5038608318346411</v>
+      </c>
+      <c r="J21" s="25">
+        <v>2.5077432000000002</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22">
-        <v>63</v>
-      </c>
-      <c r="D22">
-        <v>244787</v>
-      </c>
-      <c r="E22" s="21">
-        <f t="shared" si="0"/>
-        <v>2.83318287037037E-3</v>
-      </c>
-      <c r="F22">
-        <v>8250</v>
-      </c>
-      <c r="G22">
-        <v>15496</v>
-      </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
+      <c r="A22" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="23">
+        <v>66</v>
+      </c>
+      <c r="D22" s="23">
+        <v>323497</v>
+      </c>
+      <c r="E22" s="24">
+        <f t="shared" si="0"/>
+        <v>3.7441782407407406E-3</v>
+      </c>
+      <c r="F22" s="23">
+        <v>16480</v>
+      </c>
+      <c r="G22" s="23">
+        <v>296885</v>
+      </c>
+      <c r="H22" s="23"/>
+      <c r="I22" s="25">
+        <f>D22/(0.0117 * EXP(0.2526*C22))</f>
+        <v>1.5896463283474409</v>
+      </c>
+      <c r="J22" s="25">
+        <v>1.5949186</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23">
-        <v>64</v>
-      </c>
-      <c r="D23">
-        <v>279875</v>
-      </c>
-      <c r="E23" s="21">
-        <f t="shared" si="0"/>
-        <v>3.2392939814814815E-3</v>
-      </c>
-      <c r="F23">
-        <v>8699</v>
-      </c>
-      <c r="G23">
-        <v>17421</v>
-      </c>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
+      <c r="A23" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="23">
+        <v>66</v>
+      </c>
+      <c r="D23" s="23">
+        <v>600242</v>
+      </c>
+      <c r="E23" s="24">
+        <f t="shared" si="0"/>
+        <v>6.9472453703703701E-3</v>
+      </c>
+      <c r="F23" s="23">
+        <v>19013</v>
+      </c>
+      <c r="G23" s="23">
+        <v>569389</v>
+      </c>
+      <c r="H23" s="23"/>
+      <c r="I23" s="25">
+        <f>D23/(0.0051 * EXP(0.2674*C23))</f>
+        <v>2.5477304046671336</v>
+      </c>
+      <c r="J23" s="25">
+        <v>2.5197980000000002</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24">
-        <v>65</v>
-      </c>
-      <c r="D24">
-        <v>282665</v>
-      </c>
-      <c r="E24" s="21">
-        <f t="shared" si="0"/>
-        <v>3.271585648148148E-3</v>
-      </c>
-      <c r="F24">
-        <v>8807</v>
-      </c>
-      <c r="G24">
-        <v>17682</v>
-      </c>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
+      <c r="A24" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="23">
+        <v>66</v>
+      </c>
+      <c r="D24" s="23">
+        <v>2039310</v>
+      </c>
+      <c r="E24" s="24">
+        <f t="shared" si="0"/>
+        <v>2.3603124999999999E-2</v>
+      </c>
+      <c r="F24" s="23">
+        <v>21769</v>
+      </c>
+      <c r="G24" s="23">
+        <v>2006519</v>
+      </c>
+      <c r="H24" s="23"/>
+      <c r="I24" s="25">
+        <f>D24/(0.0013 * EXP(0.2931*C24))</f>
+        <v>6.2271146521818901</v>
+      </c>
+      <c r="J24" s="25">
+        <v>6.4888070000000004</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="4">
+      <c r="A25" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="12">
         <v>66</v>
       </c>
-      <c r="D25" s="10">
-        <v>809061</v>
+      <c r="D25" s="12">
+        <v>102443</v>
       </c>
       <c r="E25" s="20">
         <f t="shared" si="0"/>
-        <v>9.364131944444444E-3</v>
-      </c>
-      <c r="F25" s="4">
-        <v>18402</v>
-      </c>
-      <c r="G25" s="4">
-        <v>212413</v>
-      </c>
-      <c r="H25" s="14"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
+        <v>1.1856828703703704E-3</v>
+      </c>
+      <c r="F25" s="12">
+        <v>13436</v>
+      </c>
+      <c r="G25" s="12">
+        <v>82194</v>
+      </c>
+      <c r="H25" s="12"/>
+      <c r="I25" s="27">
+        <f>D25/(0.0024 * EXP(0.2812*C25))</f>
+        <v>0.37163182481165397</v>
+      </c>
+      <c r="J25" s="27">
+        <v>0.37052360000000001</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="4">
-        <v>66</v>
-      </c>
-      <c r="D26" s="10">
-        <v>595174</v>
+      <c r="A26" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="12">
+        <v>67</v>
+      </c>
+      <c r="D26" s="12">
+        <v>197416</v>
       </c>
       <c r="E26" s="20">
         <f t="shared" si="0"/>
-        <v>6.8885879629629635E-3</v>
-      </c>
-      <c r="F26" s="4">
-        <v>12560</v>
-      </c>
-      <c r="G26" s="4">
-        <v>165984</v>
-      </c>
-      <c r="H26" s="14"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
+        <v>2.2849074074074074E-3</v>
+      </c>
+      <c r="F26" s="12">
+        <v>19382</v>
+      </c>
+      <c r="G26" s="12">
+        <v>165738</v>
+      </c>
+      <c r="H26" s="12"/>
+      <c r="I26" s="27">
+        <f>D26/(0.0035 * EXP(0.2746*C26))</f>
+        <v>0.57686948545135364</v>
+      </c>
+      <c r="J26" s="27">
+        <v>0.58065900000000004</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="4">
-        <v>66</v>
-      </c>
-      <c r="D27" s="10">
-        <v>666395</v>
+      <c r="A27" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="12">
+        <v>68</v>
+      </c>
+      <c r="D27" s="12">
+        <v>478511</v>
       </c>
       <c r="E27" s="20">
         <f t="shared" si="0"/>
-        <v>7.7129050925925924E-3</v>
-      </c>
-      <c r="F27" s="4">
-        <v>15277</v>
-      </c>
-      <c r="G27" s="4">
-        <v>138154</v>
-      </c>
-      <c r="H27" s="14"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
+        <v>5.5383217592592593E-3</v>
+      </c>
+      <c r="F27" s="12">
+        <v>22334</v>
+      </c>
+      <c r="G27" s="12">
+        <v>443436</v>
+      </c>
+      <c r="H27" s="12"/>
+      <c r="I27" s="27">
+        <f>D27/(0.0033 * EXP(0.2753*C27))</f>
+        <v>1.074512734540082</v>
+      </c>
+      <c r="J27" s="27">
+        <v>1.0604889</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="4">
-        <v>66</v>
-      </c>
-      <c r="D28" s="10">
-        <v>1930064</v>
+      <c r="A28" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="12">
+        <v>69</v>
+      </c>
+      <c r="D28" s="12">
+        <v>577750</v>
       </c>
       <c r="E28" s="20">
         <f t="shared" si="0"/>
-        <v>2.2338703703703704E-2</v>
-      </c>
-      <c r="F28" s="4">
-        <v>18844</v>
-      </c>
-      <c r="G28" s="4">
-        <v>1341610</v>
-      </c>
-      <c r="H28" s="14"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
+        <v>6.6869212962962958E-3</v>
+      </c>
+      <c r="F28" s="12">
+        <v>23049</v>
+      </c>
+      <c r="G28" s="12">
+        <v>542312</v>
+      </c>
+      <c r="H28" s="12"/>
+      <c r="I28" s="27">
+        <f>D28/(0.0034 * EXP(0.2751*C28))</f>
+        <v>0.96945266996763946</v>
+      </c>
+      <c r="J28" s="27">
+        <v>0.97576700000000005</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="13">
-        <v>66</v>
-      </c>
-      <c r="D29" s="14">
-        <v>317918</v>
-      </c>
-      <c r="E29" s="21">
-        <f t="shared" si="0"/>
-        <v>3.6796064814814816E-3</v>
-      </c>
-      <c r="F29" s="13">
-        <v>9113</v>
-      </c>
-      <c r="G29" s="13">
-        <v>18467</v>
+      <c r="A29" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="12">
+        <v>70</v>
+      </c>
+      <c r="D29" s="12">
+        <v>646910</v>
+      </c>
+      <c r="E29" s="20">
+        <f t="shared" si="0"/>
+        <v>7.4873842592592596E-3</v>
+      </c>
+      <c r="F29" s="12">
+        <v>23723</v>
+      </c>
+      <c r="G29" s="12">
+        <v>608292</v>
+      </c>
+      <c r="H29" s="12"/>
+      <c r="I29" s="27">
+        <f>D29/(0.0038 * EXP(0.2732*C29))</f>
+        <v>0.84258281276942482</v>
+      </c>
+      <c r="J29" s="27">
+        <v>0.85032468000000005</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="13">
+      <c r="A30" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="D30" s="14">
-        <v>509197</v>
-      </c>
-      <c r="E30" s="21">
-        <f t="shared" si="0"/>
-        <v>5.8934837962962968E-3</v>
-      </c>
-      <c r="F30" s="13">
-        <v>13392</v>
-      </c>
-      <c r="G30" s="13">
-        <v>35294</v>
+      <c r="C30" s="23">
+        <v>71</v>
+      </c>
+      <c r="D30" s="23">
+        <v>1336053</v>
+      </c>
+      <c r="E30" s="24">
+        <f t="shared" si="0"/>
+        <v>1.5463576388888888E-2</v>
+      </c>
+      <c r="F30" s="23">
+        <v>28787</v>
+      </c>
+      <c r="G30" s="23">
+        <v>1289560</v>
+      </c>
+      <c r="H30" s="23"/>
+      <c r="I30" s="25">
+        <f>D30/(0.0032 * EXP(0.276*C30))</f>
+        <v>1.2889588147490498</v>
+      </c>
+      <c r="J30" s="25">
+        <v>1.2862548</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="13">
+      <c r="A31" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="14">
-        <v>664614</v>
-      </c>
-      <c r="E31" s="21">
-        <f t="shared" si="0"/>
-        <v>7.6922916666666667E-3</v>
-      </c>
-      <c r="F31" s="13">
-        <v>15908</v>
-      </c>
-      <c r="G31" s="13">
-        <v>55980</v>
+      <c r="C31" s="23">
+        <v>71</v>
+      </c>
+      <c r="D31" s="23">
+        <v>1819359</v>
+      </c>
+      <c r="E31" s="24">
+        <f t="shared" si="0"/>
+        <v>2.1057395833333336E-2</v>
+      </c>
+      <c r="F31" s="23">
+        <v>31196</v>
+      </c>
+      <c r="G31" s="23">
+        <v>1768305</v>
+      </c>
+      <c r="H31" s="23"/>
+      <c r="I31" s="25">
+        <f>D31/(0.0025 * EXP(0.2807*C31))</f>
+        <v>1.6092357008666069</v>
+      </c>
+      <c r="J31" s="25">
+        <v>1.640938</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="13">
+      <c r="A32" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="14">
-        <v>711559</v>
-      </c>
-      <c r="E32" s="21">
-        <f t="shared" si="0"/>
-        <v>8.235636574074074E-3</v>
-      </c>
-      <c r="F32" s="13">
-        <v>16609</v>
-      </c>
-      <c r="G32" s="13">
-        <v>59892</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="13">
+      <c r="C32" s="12">
+        <v>71</v>
+      </c>
+      <c r="D32" s="12">
+        <v>1099992</v>
+      </c>
+      <c r="E32" s="20">
+        <f t="shared" si="0"/>
+        <v>1.2731388888888889E-2</v>
+      </c>
+      <c r="F32" s="12">
+        <v>28259</v>
+      </c>
+      <c r="G32" s="12">
+        <v>1053339</v>
+      </c>
+      <c r="I32" s="27">
+        <f>D32/(0.0025 * EXP(0.2806*C32))</f>
+        <v>0.97988311202294121</v>
+      </c>
+      <c r="J32" s="27">
+        <v>0.99296366599999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="12">
+        <v>72</v>
+      </c>
+      <c r="D33" s="12">
+        <v>1477043</v>
+      </c>
+      <c r="E33" s="20">
+        <f t="shared" si="0"/>
+        <v>1.7095405092592591E-2</v>
+      </c>
+      <c r="F33" s="12">
+        <v>31079</v>
+      </c>
+      <c r="G33" s="12">
+        <v>1425694</v>
+      </c>
+      <c r="I33" s="27">
+        <f>D33/(0.0025 * EXP(0.2807*C33))</f>
+        <v>0.98670637250783955</v>
+      </c>
+      <c r="J33" s="27">
+        <v>1.006275</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="23">
+        <v>73</v>
+      </c>
+      <c r="D34" s="23">
+        <v>3875593</v>
+      </c>
+      <c r="E34" s="24">
+        <f t="shared" si="0"/>
+        <v>4.4856400462962964E-2</v>
+      </c>
+      <c r="F34" s="23">
+        <v>43977</v>
+      </c>
+      <c r="G34" s="23">
+        <v>3802535</v>
+      </c>
+      <c r="H34" s="23"/>
+      <c r="I34" s="25">
+        <f>D34/(0.0018 * EXP(0.2857*C34))</f>
+        <v>1.8852828362485301</v>
+      </c>
+      <c r="J34" s="25">
+        <v>1.84900077</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="14">
-        <v>743164</v>
-      </c>
-      <c r="E33" s="21">
-        <f t="shared" si="0"/>
-        <v>8.6014351851851859E-3</v>
-      </c>
-      <c r="F33" s="13">
-        <v>17271</v>
-      </c>
-      <c r="G33" s="13">
-        <v>64117</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="4">
+      <c r="C35" s="12">
+        <v>73</v>
+      </c>
+      <c r="D35" s="12">
+        <v>1815057</v>
+      </c>
+      <c r="E35" s="20">
+        <f t="shared" si="0"/>
+        <v>2.1007604166666666E-2</v>
+      </c>
+      <c r="F35" s="12">
+        <v>33242</v>
+      </c>
+      <c r="G35" s="12">
+        <v>1759961</v>
+      </c>
+      <c r="H35" s="12"/>
+      <c r="I35" s="27">
+        <f>D35/(0.0019 * EXP(0.2848*C35))</f>
+        <v>0.89326572583594244</v>
+      </c>
+      <c r="J35" s="27">
+        <v>0.87833018900000004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="12">
+        <v>74</v>
+      </c>
+      <c r="D36" s="12">
+        <v>1815360</v>
+      </c>
+      <c r="E36" s="20">
+        <f t="shared" si="0"/>
+        <v>2.1011111111111109E-2</v>
+      </c>
+      <c r="F36" s="12">
+        <v>35868</v>
+      </c>
+      <c r="G36" s="12">
+        <v>1755591</v>
+      </c>
+      <c r="I36" s="27">
+        <f>D36/(0.0023 * EXP(0.2821*C36))</f>
+        <v>0.67789729092217588</v>
+      </c>
+      <c r="J36" s="27">
+        <v>0.68903499000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="12">
+        <v>75</v>
+      </c>
+      <c r="D37" s="12">
+        <v>3221309</v>
+      </c>
+      <c r="E37" s="20">
+        <f t="shared" si="0"/>
+        <v>3.7283668981481478E-2</v>
+      </c>
+      <c r="F37" s="12">
+        <v>38494</v>
+      </c>
+      <c r="G37" s="12">
+        <v>3159256</v>
+      </c>
+      <c r="I37" s="27">
+        <f>D37/(0.0023 * EXP(0.2816*C37))</f>
+        <v>0.94190064035332888</v>
+      </c>
+      <c r="J37" s="27">
+        <v>0.92985499999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="12">
+        <v>76</v>
+      </c>
+      <c r="D38" s="12">
+        <v>3787043</v>
+      </c>
+      <c r="E38" s="20">
+        <f t="shared" si="0"/>
+        <v>4.3831516203703708E-2</v>
+      </c>
+      <c r="F38" s="12">
+        <v>41120</v>
+      </c>
+      <c r="G38" s="12">
+        <v>3720180</v>
+      </c>
+      <c r="I38" s="27">
+        <f>D38/(0.0025 * EXP(0.2804*C38))</f>
+        <v>0.8421144130925613</v>
+      </c>
+      <c r="J38" s="27">
+        <v>0.84155429999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="12">
+        <v>77</v>
+      </c>
+      <c r="D39" s="12">
+        <v>3994613</v>
+      </c>
+      <c r="E39" s="20">
+        <f t="shared" si="0"/>
+        <v>4.6233946759259258E-2</v>
+      </c>
+      <c r="F39" s="12">
+        <v>42315</v>
+      </c>
+      <c r="G39" s="12">
+        <v>3918822</v>
+      </c>
+      <c r="I39" s="27">
+        <f>D39/(0.0029 * EXP(0.278*C39))</f>
+        <v>0.69593556872148665</v>
+      </c>
+      <c r="J39" s="27">
+        <v>0.69922756900000005</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="12">
+        <v>78</v>
+      </c>
+      <c r="D40" s="12">
+        <v>3971849</v>
+      </c>
+      <c r="E40" s="20">
+        <f t="shared" si="0"/>
+        <v>4.5970474537037037E-2</v>
+      </c>
+      <c r="F40" s="12">
+        <v>47927</v>
+      </c>
+      <c r="G40" s="12">
+        <v>3929634</v>
+      </c>
+      <c r="I40" s="27">
+        <f>D40/(0.0036 * EXP(0.2744*C40))</f>
+        <v>0.55898296566186878</v>
+      </c>
+      <c r="J40" s="27">
+        <v>0.56305070000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="12">
+        <v>79</v>
+      </c>
+      <c r="D41" s="12">
+        <v>5258059</v>
+      </c>
+      <c r="E41" s="20">
+        <f t="shared" si="0"/>
+        <v>6.0857164351851852E-2</v>
+      </c>
+      <c r="F41" s="12">
+        <v>53497</v>
+      </c>
+      <c r="G41" s="12">
+        <v>5209173</v>
+      </c>
+      <c r="I41" s="27">
+        <f>D41/(0.0043 * EXP(0.2712*C41))</f>
+        <v>0.60629583315248625</v>
+      </c>
+      <c r="J41" s="27">
+        <v>0.60114999999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="10">
-        <v>1162769</v>
-      </c>
-      <c r="E34" s="20">
-        <f t="shared" si="0"/>
-        <v>1.3457974537037037E-2</v>
-      </c>
-      <c r="F34" s="4">
-        <v>22690</v>
-      </c>
-      <c r="G34" s="4">
-        <v>207746</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="4">
-        <v>71</v>
-      </c>
-      <c r="D35" s="10">
-        <v>1435281</v>
-      </c>
-      <c r="E35" s="20">
-        <f t="shared" si="0"/>
-        <v>1.661204861111111E-2</v>
-      </c>
-      <c r="F35" s="4">
-        <v>25294</v>
-      </c>
-      <c r="G35" s="4">
-        <v>349558</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="13">
-        <v>71</v>
-      </c>
-      <c r="D36" s="14">
-        <v>1109696</v>
-      </c>
-      <c r="E36" s="21">
-        <f t="shared" si="0"/>
-        <v>1.2843703703703704E-2</v>
-      </c>
-      <c r="F36" s="13">
-        <v>21825</v>
-      </c>
-      <c r="G36" s="13">
-        <v>155955</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" s="13">
-        <v>72</v>
-      </c>
-      <c r="D37" s="14">
-        <v>1393977</v>
-      </c>
-      <c r="E37" s="21">
-        <f>D37/3600000/24</f>
-        <v>1.6133993055555556E-2</v>
-      </c>
-      <c r="F37" s="13">
-        <v>24691</v>
-      </c>
-      <c r="G37" s="13">
-        <v>249984</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C38" s="4">
-        <v>73</v>
-      </c>
-      <c r="D38" s="4">
-        <v>2505126</v>
-      </c>
-      <c r="E38" s="20">
-        <f>D38/3600000/24</f>
-        <v>2.8994513888888889E-2</v>
-      </c>
-      <c r="F38" s="4">
-        <v>38461</v>
-      </c>
-      <c r="G38" s="4">
-        <v>700271</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" s="13">
-        <v>73</v>
-      </c>
-      <c r="D39" s="13">
-        <v>1614447</v>
-      </c>
-      <c r="E39" s="21">
-        <f t="shared" ref="E39:E46" si="1">D39/3600000/24</f>
-        <v>1.8685729166666668E-2</v>
-      </c>
-      <c r="F39" s="13">
-        <v>26982</v>
-      </c>
-      <c r="G39" s="13">
-        <v>325120</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C40" s="13">
-        <v>74</v>
-      </c>
-      <c r="D40">
-        <v>1940835</v>
-      </c>
-      <c r="E40" s="21">
-        <f t="shared" si="1"/>
-        <v>2.2463368055555558E-2</v>
-      </c>
-      <c r="F40" s="13">
-        <v>29031</v>
-      </c>
-      <c r="G40" s="13">
-        <v>411064</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" s="13">
-        <v>75</v>
-      </c>
-      <c r="D41">
-        <v>2114103</v>
-      </c>
-      <c r="E41" s="21">
-        <f t="shared" si="1"/>
-        <v>2.4468784722222223E-2</v>
-      </c>
-      <c r="F41" s="13">
-        <v>31080</v>
-      </c>
-      <c r="G41" s="13">
-        <v>491724</v>
-      </c>
-      <c r="H41" s="21"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="13">
-        <v>76</v>
-      </c>
-      <c r="D42">
-        <v>2364937</v>
-      </c>
-      <c r="E42" s="21">
-        <f t="shared" si="1"/>
-        <v>2.7371956018518519E-2</v>
-      </c>
-      <c r="F42" s="13">
-        <v>33129</v>
-      </c>
-      <c r="G42" s="13">
-        <v>611868</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C43" s="13">
-        <v>77</v>
-      </c>
-      <c r="D43">
-        <v>2555695</v>
-      </c>
-      <c r="E43" s="21">
-        <f t="shared" si="1"/>
-        <v>2.9579803240740738E-2</v>
-      </c>
-      <c r="F43" s="13">
-        <v>33899</v>
-      </c>
-      <c r="G43" s="13">
-        <v>626432</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44" s="4">
-        <v>78</v>
-      </c>
-      <c r="D44" s="10">
-        <v>3305786</v>
-      </c>
-      <c r="E44" s="20">
-        <f t="shared" si="1"/>
-        <v>3.8261412037037035E-2</v>
-      </c>
-      <c r="F44" s="4">
-        <v>38749</v>
-      </c>
-      <c r="G44" s="4">
-        <v>1002787</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C45" s="13">
-        <v>78</v>
-      </c>
-      <c r="D45" s="9"/>
-      <c r="E45" s="21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="16">
-        <v>82</v>
-      </c>
-      <c r="D46" s="17">
-        <v>15776143.311657</v>
-      </c>
-      <c r="E46" s="22">
-        <f t="shared" si="1"/>
-        <v>0.1825942512923264</v>
-      </c>
-      <c r="F46" s="16">
-        <v>89411</v>
-      </c>
-      <c r="G46" s="16">
-        <v>9528224</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
+      <c r="E42" s="14">
+        <f>SUM(E2:E41)</f>
+        <v>0.45847831018518515</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Time added as property of PlotPoints Time added for last completed subset process on GUI Key added on GUI New tab for Probability analysis added
</commit_message>
<xml_diff>
--- a/ProcessingTimeExtrapolation.xlsx
+++ b/ProcessingTimeExtrapolation.xlsx
@@ -13,7 +13,6 @@
     <sheet name="Forest1 Processing Automated" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -397,7 +396,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -487,7 +485,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1213,7 +1210,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1331,7 +1327,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1437,7 +1432,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2003,6 +1997,326 @@
         <c:axId val="556485632"/>
         <c:axId val="556488256"/>
       </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Forest1 Processing Automated'!$C$2:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>79</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Forest1 Processing Automated'!$F$2:$F$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2078</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2214</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2272</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9312</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2340</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2480</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4612</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6526</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5296</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6208</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5882</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6740</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7938</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8598</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10040</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12034</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12962</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13060</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21628</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16480</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>19013</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21769</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>13436</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>19382</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>22334</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>23049</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>23723</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28787</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>31196</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>28259</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31079</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>43977</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33242</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35868</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>38494</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>41120</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42315</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>47927</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>53497</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D447-411C-ADE8-AA14C9A2E9D5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="367730288"/>
+        <c:axId val="367724712"/>
+      </c:scatterChart>
       <c:valAx>
         <c:axId val="556485632"/>
         <c:scaling>
@@ -2126,6 +2440,69 @@
         </c:txPr>
         <c:crossAx val="556485632"/>
         <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="367724712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="60000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="367730288"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="367730288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="367724712"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -3333,7 +3710,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9282839" cy="6054025"/>
+    <xdr:ext cx="9290911" cy="6045953"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3665,7 +4042,7 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
@@ -4815,7 +5192,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L50" sqref="L50"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6091,6 +6468,14 @@
         <f>SUM(E2:E41)</f>
         <v>0.45847831018518515</v>
       </c>
+      <c r="G42">
+        <f>SUM(G2:G41)</f>
+        <v>38459140</v>
+      </c>
+      <c r="H42" s="20">
+        <f>G42/3600000/24</f>
+        <v>0.4451289351851852</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed issue in Problem Species where next dataset files were being generated incorrectly when non-sequential species were in the dataset, i.e. some species were missing Probability tab functional. Still need to ensure probabilities are calculated correctly when a set size does not have results with every subset used.
</commit_message>
<xml_diff>
--- a/ProcessingTimeExtrapolation.xlsx
+++ b/ProcessingTimeExtrapolation.xlsx
@@ -10,7 +10,8 @@
     <sheet name="Chart Manual" sheetId="2" r:id="rId1"/>
     <sheet name="Forest1 Processing Manual" sheetId="3" r:id="rId2"/>
     <sheet name="Chart Auto" sheetId="5" r:id="rId3"/>
-    <sheet name="Forest1 Processing Automated" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
+    <sheet name="Forest1 Processing Automated" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="76">
   <si>
     <t>No Species</t>
   </si>
@@ -244,6 +245,12 @@
   </si>
   <si>
     <t>Additional Test</t>
+  </si>
+  <si>
+    <t>Species ID</t>
+  </si>
+  <si>
+    <t>Set Size</t>
   </si>
 </sst>
 </file>
@@ -253,8 +260,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -300,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -339,6 +354,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2503,6 +2524,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="367724712"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -3672,7 +3694,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="141" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5188,11 +5210,144 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="28"/>
+      <c r="B2" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="29">
+        <v>3</v>
+      </c>
+      <c r="C3" s="29">
+        <v>4</v>
+      </c>
+      <c r="D3" s="29">
+        <v>5</v>
+      </c>
+      <c r="E3" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="29">
+        <v>1</v>
+      </c>
+      <c r="B4" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="28">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="29">
+        <v>2</v>
+      </c>
+      <c r="B5" s="28">
+        <v>0.17</v>
+      </c>
+      <c r="C5" s="28">
+        <v>0.05</v>
+      </c>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="29">
+        <v>3</v>
+      </c>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="29">
+        <v>4</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="29">
+        <v>5</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="29">
+        <v>6</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="29">
+        <v>7</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="29">
+        <v>8</v>
+      </c>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="29">
+        <v>9</v>
+      </c>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Probabilities calculated correctly now Cancel button added for probs tab Delete Files buttons added
</commit_message>
<xml_diff>
--- a/ProcessingTimeExtrapolation.xlsx
+++ b/ProcessingTimeExtrapolation.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="134">
   <si>
     <t>No Species</t>
   </si>
@@ -251,6 +251,180 @@
   </si>
   <si>
     <t>Set Size</t>
+  </si>
+  <si>
+    <t>50:31.33:[24, 70, 77]]</t>
+  </si>
+  <si>
+    <t>54:41.33:[24, 72, 76]]</t>
+  </si>
+  <si>
+    <t>54:41.33:[24, 72, 77]]</t>
+  </si>
+  <si>
+    <t>50:31.33:[24, 70, 77]</t>
+  </si>
+  <si>
+    <t>54:41.33:[24, 72, 76]</t>
+  </si>
+  <si>
+    <t>24,70,72,76,77</t>
+  </si>
+  <si>
+    <t>Possibly not ignoring cases where no set of size 3 exists</t>
+  </si>
+  <si>
+    <t>Probs for set size: 3</t>
+  </si>
+  <si>
+    <t>Species 70: 0.25</t>
+  </si>
+  <si>
+    <t>Species 24: 0.3582089552238806</t>
+  </si>
+  <si>
+    <t>Species 72: 0.4</t>
+  </si>
+  <si>
+    <t>Species 76: 0.26666666666666666</t>
+  </si>
+  <si>
+    <t>Species 77: 0.5</t>
+  </si>
+  <si>
+    <t>Probs for set size: 4</t>
+  </si>
+  <si>
+    <t>Species 32: 1.0</t>
+  </si>
+  <si>
+    <t>Species 33: 0.25</t>
+  </si>
+  <si>
+    <t>Species 2: 0.5</t>
+  </si>
+  <si>
+    <t>Species 3: 0.5</t>
+  </si>
+  <si>
+    <t>Species 70: 0.6666666666666666</t>
+  </si>
+  <si>
+    <t>Species 72: 0.6666666666666666</t>
+  </si>
+  <si>
+    <t>Species 8: 0.6666666666666666</t>
+  </si>
+  <si>
+    <t>Species 47: 0.25</t>
+  </si>
+  <si>
+    <t>Species 16: 0.3333333333333333</t>
+  </si>
+  <si>
+    <t>Species 80: 0.2</t>
+  </si>
+  <si>
+    <t>Species 17: 0.5</t>
+  </si>
+  <si>
+    <t>Species 81: 0.16666666666666666</t>
+  </si>
+  <si>
+    <t>Species 50: 0.4</t>
+  </si>
+  <si>
+    <t>Species 18: 0.5</t>
+  </si>
+  <si>
+    <t>Species 19: 0.5</t>
+  </si>
+  <si>
+    <t>Species 84: 0.6</t>
+  </si>
+  <si>
+    <t>Species 85: 0.6666666666666666</t>
+  </si>
+  <si>
+    <t>Species 86: 0.3333333333333333</t>
+  </si>
+  <si>
+    <t>Species 87: 0.4</t>
+  </si>
+  <si>
+    <t>Species 24: 1.0</t>
+  </si>
+  <si>
+    <t>Species 25: 0.8</t>
+  </si>
+  <si>
+    <t>Species 60: 0.4</t>
+  </si>
+  <si>
+    <t>Species 61: 0.16666666666666666</t>
+  </si>
+  <si>
+    <t>54:26.00:[25, 33, 61, 72]</t>
+  </si>
+  <si>
+    <t>54:26.00:[25, 50, 61, 72]</t>
+  </si>
+  <si>
+    <t>24:18.00:[25, 50, 60, 70]</t>
+  </si>
+  <si>
+    <t>24:18.00:[25, 60, 70, 87]</t>
+  </si>
+  <si>
+    <t>54:25.50:[2, 24, 47, 72]</t>
+  </si>
+  <si>
+    <t>22:17.00:[19, 25, 32, 80]</t>
+  </si>
+  <si>
+    <t>20:18.50:[2, 18, 24, 84]</t>
+  </si>
+  <si>
+    <t>20:17.00:[3, 16, 24, 85]</t>
+  </si>
+  <si>
+    <t>20:18.50:[3, 8, 24, 84]</t>
+  </si>
+  <si>
+    <t>20:18.50:[3, 8, 24, 86]</t>
+  </si>
+  <si>
+    <t>20:18.50:[3, 17, 24, 84]</t>
+  </si>
+  <si>
+    <t>20:18.50:[3, 17, 24, 86]</t>
+  </si>
+  <si>
+    <t>24:18.75:[8, 24, 81, 87]</t>
+  </si>
+  <si>
+    <t>24:18.75:[17, 24, 81, 87]</t>
+  </si>
+  <si>
+    <t>20:19.00:[3, 18, 24, 84]</t>
+  </si>
+  <si>
+    <t>20:19.00:[3, 18, 24, 85]</t>
+  </si>
+  <si>
+    <t>20:19.00:[3, 19, 24, 84]</t>
+  </si>
+  <si>
+    <t>20:19.00:[3, 19, 24, 85]</t>
+  </si>
+  <si>
+    <t>24:17.00:[25, 32, 60, 70]</t>
+  </si>
+  <si>
+    <t>Appearances</t>
+  </si>
+  <si>
+    <t>Probability</t>
   </si>
 </sst>
 </file>
@@ -3694,7 +3868,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="141" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5210,18 +5384,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E12"/>
+  <dimension ref="A2:AD61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="30" customWidth="1"/>
+    <col min="8" max="15" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="33" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="28"/>
       <c r="B2" s="28" t="s">
         <v>75</v>
@@ -5230,7 +5409,7 @@
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>74</v>
       </c>
@@ -5247,7 +5426,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="29">
         <v>1</v>
       </c>
@@ -5260,7 +5439,7 @@
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="29">
         <v>2</v>
       </c>
@@ -5273,7 +5452,7 @@
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
         <v>3</v>
       </c>
@@ -5282,7 +5461,7 @@
       <c r="D6" s="28"/>
       <c r="E6" s="28"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="29">
         <v>4</v>
       </c>
@@ -5291,7 +5470,7 @@
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <v>5</v>
       </c>
@@ -5300,7 +5479,7 @@
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <v>6</v>
       </c>
@@ -5309,7 +5488,7 @@
       <c r="D9" s="28"/>
       <c r="E9" s="28"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
         <v>7</v>
       </c>
@@ -5318,7 +5497,7 @@
       <c r="D10" s="28"/>
       <c r="E10" s="28"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
         <v>8</v>
       </c>
@@ -5327,7 +5506,7 @@
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>9</v>
       </c>
@@ -5335,6 +5514,862 @@
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
       <c r="E12" s="28"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="29">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="29">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="29">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="29">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="29">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="29">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="29">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="29">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="29">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="29">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="29">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="29">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="29">
+        <v>69</v>
+      </c>
+      <c r="B26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="29">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="29">
+        <v>75</v>
+      </c>
+      <c r="B28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="29">
+        <v>76</v>
+      </c>
+      <c r="B29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="29">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="29">
+        <v>90</v>
+      </c>
+      <c r="B31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="29">
+        <v>83</v>
+      </c>
+      <c r="B32" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A33" s="29">
+        <v>87</v>
+      </c>
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A34" s="29">
+        <v>93</v>
+      </c>
+      <c r="B34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A35" s="29">
+        <v>95</v>
+      </c>
+      <c r="B35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A36" s="29">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>3</v>
+      </c>
+      <c r="J37">
+        <v>8</v>
+      </c>
+      <c r="K37">
+        <v>16</v>
+      </c>
+      <c r="L37">
+        <v>17</v>
+      </c>
+      <c r="M37">
+        <v>18</v>
+      </c>
+      <c r="N37">
+        <v>19</v>
+      </c>
+      <c r="O37">
+        <v>24</v>
+      </c>
+      <c r="P37">
+        <v>25</v>
+      </c>
+      <c r="Q37">
+        <v>32</v>
+      </c>
+      <c r="R37">
+        <v>33</v>
+      </c>
+      <c r="S37">
+        <v>47</v>
+      </c>
+      <c r="T37">
+        <v>50</v>
+      </c>
+      <c r="U37">
+        <v>60</v>
+      </c>
+      <c r="V37">
+        <v>61</v>
+      </c>
+      <c r="W37">
+        <v>70</v>
+      </c>
+      <c r="X37">
+        <v>72</v>
+      </c>
+      <c r="Y37">
+        <v>80</v>
+      </c>
+      <c r="Z37">
+        <v>81</v>
+      </c>
+      <c r="AA37">
+        <v>84</v>
+      </c>
+      <c r="AB37">
+        <v>85</v>
+      </c>
+      <c r="AC37">
+        <v>86</v>
+      </c>
+      <c r="AD37">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A38" s="29">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>131</v>
+      </c>
+      <c r="F38" t="s">
+        <v>89</v>
+      </c>
+      <c r="P38">
+        <v>1</v>
+      </c>
+      <c r="Q38">
+        <v>1</v>
+      </c>
+      <c r="U38">
+        <v>1</v>
+      </c>
+      <c r="W38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A39" s="29">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" t="s">
+        <v>114</v>
+      </c>
+      <c r="F39" t="s">
+        <v>92</v>
+      </c>
+      <c r="P39">
+        <v>1</v>
+      </c>
+      <c r="R39">
+        <v>1</v>
+      </c>
+      <c r="T39">
+        <v>1</v>
+      </c>
+      <c r="V39">
+        <v>1</v>
+      </c>
+      <c r="X39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A40" s="29">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>127</v>
+      </c>
+      <c r="C40" t="s">
+        <v>128</v>
+      </c>
+      <c r="D40" t="s">
+        <v>129</v>
+      </c>
+      <c r="E40" t="s">
+        <v>130</v>
+      </c>
+      <c r="F40" t="s">
+        <v>93</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <v>1</v>
+      </c>
+      <c r="AA40">
+        <v>1</v>
+      </c>
+      <c r="AB40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A41" s="29">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" t="s">
+        <v>122</v>
+      </c>
+      <c r="D41" t="s">
+        <v>123</v>
+      </c>
+      <c r="E41" t="s">
+        <v>124</v>
+      </c>
+      <c r="F41" t="s">
+        <v>96</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="O41">
+        <v>1</v>
+      </c>
+      <c r="AA41">
+        <v>1</v>
+      </c>
+      <c r="AC41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A42" s="29">
+        <v>4</v>
+      </c>
+      <c r="B42" t="s">
+        <v>120</v>
+      </c>
+      <c r="F42" t="s">
+        <v>98</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="O42">
+        <v>1</v>
+      </c>
+      <c r="AB42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A43" s="29">
+        <v>5</v>
+      </c>
+      <c r="B43" t="s">
+        <v>119</v>
+      </c>
+      <c r="F43" t="s">
+        <v>100</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="O43">
+        <v>1</v>
+      </c>
+      <c r="AA43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A44" s="29">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>118</v>
+      </c>
+      <c r="F44" t="s">
+        <v>103</v>
+      </c>
+      <c r="N44">
+        <v>1</v>
+      </c>
+      <c r="P44">
+        <v>1</v>
+      </c>
+      <c r="Q44">
+        <v>1</v>
+      </c>
+      <c r="Y44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A45" s="29">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s">
+        <v>117</v>
+      </c>
+      <c r="F45" t="s">
+        <v>104</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="O45">
+        <v>1</v>
+      </c>
+      <c r="S45">
+        <v>1</v>
+      </c>
+      <c r="X45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A46" s="29">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" t="s">
+        <v>116</v>
+      </c>
+      <c r="F46" t="s">
+        <v>109</v>
+      </c>
+      <c r="P46">
+        <v>1</v>
+      </c>
+      <c r="T46">
+        <v>1</v>
+      </c>
+      <c r="U46">
+        <v>1</v>
+      </c>
+      <c r="W46">
+        <v>1</v>
+      </c>
+      <c r="AD46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A47" s="29">
+        <v>9</v>
+      </c>
+      <c r="B47" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" t="s">
+        <v>126</v>
+      </c>
+      <c r="F47" t="s">
+        <v>110</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+      <c r="Z47">
+        <v>1</v>
+      </c>
+      <c r="AD47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>91</v>
+      </c>
+      <c r="H49">
+        <f>SUM(H38:H47)</f>
+        <v>2</v>
+      </c>
+      <c r="I49">
+        <f t="shared" ref="I49:AD49" si="0">SUM(I38:I47)</f>
+        <v>3</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="R49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T49">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U49">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="V49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W49">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="X49">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Y49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Z49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AA49">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AB49">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AC49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AD49">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>97</v>
+      </c>
+      <c r="G50" t="s">
+        <v>132</v>
+      </c>
+      <c r="H50">
+        <v>4</v>
+      </c>
+      <c r="I50">
+        <v>6</v>
+      </c>
+      <c r="J50">
+        <v>3</v>
+      </c>
+      <c r="K50">
+        <v>3</v>
+      </c>
+      <c r="L50">
+        <v>4</v>
+      </c>
+      <c r="M50">
+        <v>4</v>
+      </c>
+      <c r="N50">
+        <v>4</v>
+      </c>
+      <c r="O50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>102</v>
+      </c>
+      <c r="G51" t="s">
+        <v>133</v>
+      </c>
+      <c r="H51" s="8">
+        <f>H49/H50</f>
+        <v>0.5</v>
+      </c>
+      <c r="I51" s="8">
+        <f t="shared" ref="I51:AD51" si="1">I49/I50</f>
+        <v>0.5</v>
+      </c>
+      <c r="J51" s="8">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K51" s="8">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L51" s="8">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="M51" s="8">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="N51" s="8">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="O51" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P51" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q51" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R51" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S51" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T51" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U51" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V51" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W51" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X51" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y51" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Z51" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AA51" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB51" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC51" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD51" s="8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="55" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="60" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F61" t="s">
+        <v>108</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5346,7 +6381,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added SpecSelException Various tidying up and bug fixing Allow saving probabilties data to specified file
</commit_message>
<xml_diff>
--- a/ProcessingTimeExtrapolation.xlsx
+++ b/ProcessingTimeExtrapolation.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="106">
   <si>
     <t>No Species</t>
   </si>
@@ -295,136 +295,52 @@
     <t>Probs for set size: 4</t>
   </si>
   <si>
-    <t>Species 32: 1.0</t>
-  </si>
-  <si>
-    <t>Species 33: 0.25</t>
-  </si>
-  <si>
-    <t>Species 2: 0.5</t>
-  </si>
-  <si>
-    <t>Species 3: 0.5</t>
-  </si>
-  <si>
-    <t>Species 70: 0.6666666666666666</t>
-  </si>
-  <si>
-    <t>Species 72: 0.6666666666666666</t>
-  </si>
-  <si>
-    <t>Species 8: 0.6666666666666666</t>
-  </si>
-  <si>
-    <t>Species 47: 0.25</t>
-  </si>
-  <si>
-    <t>Species 16: 0.3333333333333333</t>
-  </si>
-  <si>
-    <t>Species 80: 0.2</t>
-  </si>
-  <si>
-    <t>Species 17: 0.5</t>
-  </si>
-  <si>
-    <t>Species 81: 0.16666666666666666</t>
-  </si>
-  <si>
-    <t>Species 50: 0.4</t>
-  </si>
-  <si>
-    <t>Species 18: 0.5</t>
-  </si>
-  <si>
-    <t>Species 19: 0.5</t>
-  </si>
-  <si>
-    <t>Species 84: 0.6</t>
-  </si>
-  <si>
-    <t>Species 85: 0.6666666666666666</t>
-  </si>
-  <si>
-    <t>Species 86: 0.3333333333333333</t>
-  </si>
-  <si>
-    <t>Species 87: 0.4</t>
-  </si>
-  <si>
-    <t>Species 24: 1.0</t>
-  </si>
-  <si>
-    <t>Species 25: 0.8</t>
-  </si>
-  <si>
-    <t>Species 60: 0.4</t>
-  </si>
-  <si>
-    <t>Species 61: 0.16666666666666666</t>
-  </si>
-  <si>
-    <t>54:26.00:[25, 33, 61, 72]</t>
-  </si>
-  <si>
-    <t>54:26.00:[25, 50, 61, 72]</t>
-  </si>
-  <si>
-    <t>24:18.00:[25, 50, 60, 70]</t>
-  </si>
-  <si>
-    <t>24:18.00:[25, 60, 70, 87]</t>
-  </si>
-  <si>
-    <t>54:25.50:[2, 24, 47, 72]</t>
-  </si>
-  <si>
-    <t>22:17.00:[19, 25, 32, 80]</t>
-  </si>
-  <si>
-    <t>20:18.50:[2, 18, 24, 84]</t>
-  </si>
-  <si>
-    <t>20:17.00:[3, 16, 24, 85]</t>
-  </si>
-  <si>
-    <t>20:18.50:[3, 8, 24, 84]</t>
-  </si>
-  <si>
-    <t>20:18.50:[3, 8, 24, 86]</t>
-  </si>
-  <si>
-    <t>20:18.50:[3, 17, 24, 84]</t>
-  </si>
-  <si>
-    <t>20:18.50:[3, 17, 24, 86]</t>
-  </si>
-  <si>
-    <t>24:18.75:[8, 24, 81, 87]</t>
-  </si>
-  <si>
-    <t>24:18.75:[17, 24, 81, 87]</t>
-  </si>
-  <si>
     <t>20:19.00:[3, 18, 24, 84]</t>
   </si>
   <si>
-    <t>20:19.00:[3, 18, 24, 85]</t>
-  </si>
-  <si>
     <t>20:19.00:[3, 19, 24, 84]</t>
   </si>
   <si>
-    <t>20:19.00:[3, 19, 24, 85]</t>
-  </si>
-  <si>
-    <t>24:17.00:[25, 32, 60, 70]</t>
-  </si>
-  <si>
     <t>Appearances</t>
   </si>
   <si>
     <t>Probability</t>
+  </si>
+  <si>
+    <t>Species:     3    7    8   17   18   19   23   24   25   33   35   49   50   52   58   70   78   80   81   83   84   88</t>
+  </si>
+  <si>
+    <t>Probs  :     1 0.33 0.75 0.33 0.33 0.67 0.33    1 0.67 0.75 0.25 0.33    1 0.33 0.25 0.67  0.5  0.5 0.33 0.17  0.2  0.5</t>
+  </si>
+  <si>
+    <t>24:18.75:[8, 24, 33, 81]</t>
+  </si>
+  <si>
+    <t>24:18.75:[17, 24, 33, 81]</t>
+  </si>
+  <si>
+    <t>22:19.00:[7, 24, 49, 80]</t>
+  </si>
+  <si>
+    <t>36:21.00:[8, 24, 78, 88]</t>
+  </si>
+  <si>
+    <t>36:21.75:[8, 24, 33, 78]</t>
+  </si>
+  <si>
+    <t>36:21.75:[8, 24, 50, 78]</t>
+  </si>
+  <si>
+    <t>24:19.00:[24, 33, 35, 70]</t>
+  </si>
+  <si>
+    <t>24:17.00:[23, 25, 58, 70]</t>
+  </si>
+  <si>
+    <t>24:17.00:[25, 58, 70, 88]</t>
+  </si>
+  <si>
+    <t>48:24.00:[19, 25, 52, 83]</t>
   </si>
 </sst>
 </file>
@@ -1808,7 +1724,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1885,7 +1800,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -5384,10 +5298,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AD61"/>
+  <dimension ref="A2:AD72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5697,7 +5611,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="29">
         <v>87</v>
       </c>
@@ -5708,7 +5622,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="29">
         <v>93</v>
       </c>
@@ -5719,7 +5633,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="29">
         <v>95</v>
       </c>
@@ -5730,7 +5644,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="29">
         <v>97</v>
       </c>
@@ -5738,27 +5652,27 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H37">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I37">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J37">
         <v>8</v>
       </c>
       <c r="K37">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L37">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M37">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N37">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="O37">
         <v>24</v>
@@ -5767,28 +5681,28 @@
         <v>25</v>
       </c>
       <c r="Q37">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R37">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="S37">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="T37">
         <v>50</v>
       </c>
       <c r="U37">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="V37">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="W37">
         <v>70</v>
       </c>
       <c r="X37">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="Y37">
         <v>80</v>
@@ -5797,468 +5711,318 @@
         <v>81</v>
       </c>
       <c r="AA37">
+        <v>83</v>
+      </c>
+      <c r="AB37">
         <v>84</v>
       </c>
-      <c r="AB37">
-        <v>85</v>
-      </c>
       <c r="AC37">
-        <v>86</v>
-      </c>
-      <c r="AD37">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="29">
         <v>0</v>
       </c>
-      <c r="B38" t="s">
-        <v>131</v>
-      </c>
-      <c r="F38" t="s">
-        <v>89</v>
-      </c>
-      <c r="P38">
-        <v>1</v>
-      </c>
-      <c r="Q38">
-        <v>1</v>
-      </c>
-      <c r="U38">
-        <v>1</v>
-      </c>
-      <c r="W38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="29">
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="C39" t="s">
-        <v>114</v>
-      </c>
-      <c r="F39" t="s">
-        <v>92</v>
-      </c>
-      <c r="P39">
+        <v>97</v>
+      </c>
+      <c r="J39">
         <v>1</v>
       </c>
-      <c r="R39">
+      <c r="K39">
         <v>1</v>
       </c>
-      <c r="T39">
+      <c r="O39">
         <v>1</v>
       </c>
-      <c r="V39">
+      <c r="Q39">
         <v>1</v>
       </c>
-      <c r="X39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="29">
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>127</v>
-      </c>
-      <c r="C40" t="s">
-        <v>128</v>
-      </c>
-      <c r="D40" t="s">
-        <v>129</v>
-      </c>
-      <c r="E40" t="s">
-        <v>130</v>
-      </c>
-      <c r="F40" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="I40">
         <v>1</v>
       </c>
-      <c r="M40">
-        <v>1</v>
-      </c>
-      <c r="N40">
-        <v>1</v>
-      </c>
       <c r="O40">
         <v>1</v>
       </c>
-      <c r="AA40">
+      <c r="S40">
         <v>1</v>
       </c>
-      <c r="AB40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="29">
         <v>3</v>
       </c>
-      <c r="B41" t="s">
-        <v>121</v>
-      </c>
-      <c r="C41" t="s">
-        <v>122</v>
-      </c>
-      <c r="D41" t="s">
-        <v>123</v>
-      </c>
-      <c r="E41" t="s">
-        <v>124</v>
-      </c>
-      <c r="F41" t="s">
-        <v>96</v>
-      </c>
-      <c r="I41">
-        <v>1</v>
-      </c>
-      <c r="J41">
-        <v>1</v>
-      </c>
-      <c r="L41">
-        <v>1</v>
-      </c>
-      <c r="O41">
-        <v>1</v>
-      </c>
-      <c r="AA41">
-        <v>1</v>
-      </c>
-      <c r="AC41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42" s="29">
         <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>120</v>
-      </c>
-      <c r="F42" t="s">
-        <v>98</v>
-      </c>
-      <c r="I42">
-        <v>1</v>
-      </c>
-      <c r="K42">
+        <v>99</v>
+      </c>
+      <c r="J42">
         <v>1</v>
       </c>
       <c r="O42">
         <v>1</v>
       </c>
-      <c r="AB42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A43" s="29">
         <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>119</v>
-      </c>
-      <c r="F43" t="s">
         <v>100</v>
       </c>
-      <c r="H43">
-        <v>1</v>
-      </c>
-      <c r="M43">
+      <c r="C43" t="s">
+        <v>101</v>
+      </c>
+      <c r="J43">
         <v>1</v>
       </c>
       <c r="O43">
         <v>1</v>
       </c>
-      <c r="AA43">
+      <c r="Q43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A44" s="29">
         <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>118</v>
-      </c>
-      <c r="F44" t="s">
-        <v>103</v>
-      </c>
-      <c r="N44">
-        <v>1</v>
-      </c>
-      <c r="P44">
+        <v>102</v>
+      </c>
+      <c r="O44">
         <v>1</v>
       </c>
       <c r="Q44">
         <v>1</v>
       </c>
-      <c r="Y44">
+      <c r="R44">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A45" s="29">
         <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>117</v>
-      </c>
-      <c r="F45" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45" t="s">
         <v>104</v>
       </c>
-      <c r="H45">
+      <c r="N45">
         <v>1</v>
       </c>
-      <c r="O45">
+      <c r="P45">
         <v>1</v>
       </c>
-      <c r="S45">
+      <c r="V45">
         <v>1</v>
       </c>
-      <c r="X45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A46" s="29">
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>115</v>
-      </c>
-      <c r="C46" t="s">
-        <v>116</v>
-      </c>
-      <c r="F46" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="M46">
+        <v>1</v>
       </c>
       <c r="P46">
         <v>1</v>
       </c>
-      <c r="T46">
-        <v>1</v>
-      </c>
       <c r="U46">
         <v>1</v>
       </c>
-      <c r="W46">
-        <v>1</v>
-      </c>
-      <c r="AD46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A47" s="29">
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="C47" t="s">
-        <v>126</v>
-      </c>
-      <c r="F47" t="s">
-        <v>110</v>
-      </c>
-      <c r="J47">
+        <v>91</v>
+      </c>
+      <c r="H47">
         <v>1</v>
       </c>
       <c r="L47">
         <v>1</v>
       </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
       <c r="O47">
         <v>1</v>
       </c>
-      <c r="Z47">
-        <v>1</v>
-      </c>
-      <c r="AD47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="F48" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F49" t="s">
-        <v>91</v>
-      </c>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
       <c r="H49">
         <f>SUM(H38:H47)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I49">
         <f t="shared" ref="I49:AD49" si="0">SUM(I38:I47)</f>
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="J49">
+      <c r="K49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M49">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="K49">
+      <c r="N49">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L49">
+      <c r="O49">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="P49">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="M49">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="N49">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="O49">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="P49">
-        <f t="shared" si="0"/>
+      <c r="Q49">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="R49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="V49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AC49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>92</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>3</v>
+      </c>
+      <c r="J50">
         <v>4</v>
       </c>
-      <c r="Q49">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="R49">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="S49">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="T49">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="U49">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="V49">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="W49">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="X49">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="Y49">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="Z49">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AA49">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="AB49">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="AC49">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AD49">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F50" t="s">
-        <v>97</v>
-      </c>
-      <c r="G50" t="s">
-        <v>132</v>
-      </c>
-      <c r="H50">
-        <v>4</v>
-      </c>
-      <c r="I50">
-        <v>6</v>
-      </c>
-      <c r="J50">
-        <v>3</v>
-      </c>
-      <c r="K50">
-        <v>3</v>
-      </c>
-      <c r="L50">
-        <v>4</v>
-      </c>
-      <c r="M50">
-        <v>4</v>
-      </c>
-      <c r="N50">
-        <v>4</v>
-      </c>
-      <c r="O50">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F51" t="s">
-        <v>102</v>
-      </c>
+    </row>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="H51" s="8">
         <f>H49/H50</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I51" s="8">
         <f t="shared" ref="I51:AD51" si="1">I49/I50</f>
-        <v>0.5</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J51" s="8">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="K51" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="K51" s="8" t="e">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="L51" s="8">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L51" s="8" t="e">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="M51" s="8">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M51" s="8" t="e">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="N51" s="8">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N51" s="8" t="e">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="O51" s="8">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O51" s="8" t="e">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P51" s="8" t="e">
         <f t="shared" si="1"/>
@@ -6316,59 +6080,86 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD51" s="8" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="52" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F52" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="53" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F53" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="54" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F54" t="s">
+      <c r="AD51" s="8"/>
+    </row>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="55" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F55" t="s">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F56" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="57" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F57" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="58" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F58" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="59" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F59" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="60" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F60" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="61" spans="6:30" x14ac:dyDescent="0.25">
-      <c r="F61" t="s">
-        <v>108</v>
+    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A63" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A64" s="29">
+        <v>1</v>
+      </c>
+      <c r="B64" t="s">
+        <v>80</v>
+      </c>
+      <c r="C64" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="29">
+        <v>5</v>
+      </c>
+      <c r="B68" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="29">
+        <v>6</v>
+      </c>
+      <c r="B69" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="29">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>